<commit_message>
added more metadata incorporation
</commit_message>
<xml_diff>
--- a/data/atlas_project_metadata.xlsx
+++ b/data/atlas_project_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbernabei/Documents/PhD_Research/atlas_project/iEEG_atlas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2436D952-002F-5146-9075-B3948C5B1DC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21323ED-AF3F-9147-AFDF-B042DE7D1766}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8340" yWindow="1920" windowWidth="25260" windowHeight="17720" xr2:uid="{55386E59-C2B1-FE47-8A03-2662CFD6A014}"/>
+    <workbookView xWindow="16360" yWindow="2120" windowWidth="25260" windowHeight="17720" xr2:uid="{55386E59-C2B1-FE47-8A03-2662CFD6A014}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -558,15 +558,6 @@
     <t>Hypothesis 2</t>
   </si>
   <si>
-    <t>Lesion status</t>
-  </si>
-  <si>
-    <t>Age onset</t>
-  </si>
-  <si>
-    <t>Age surgery</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -631,6 +622,15 @@
   </si>
   <si>
     <t>Insular</t>
+  </si>
+  <si>
+    <t>Lesion_status</t>
+  </si>
+  <si>
+    <t>Age_onset</t>
+  </si>
+  <si>
+    <t>Age_surgery</t>
   </si>
 </sst>
 </file>
@@ -984,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEE15CE-15A7-E440-8B77-868E4F33ECBC}">
   <dimension ref="A1:S86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1044,19 +1044,19 @@
         <v>76</v>
       </c>
       <c r="L1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="M1" t="s">
+        <v>199</v>
+      </c>
+      <c r="N1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O1" t="s">
+        <v>201</v>
+      </c>
+      <c r="P1" t="s">
         <v>177</v>
-      </c>
-      <c r="N1" t="s">
-        <v>178</v>
-      </c>
-      <c r="O1" t="s">
-        <v>179</v>
-      </c>
-      <c r="P1" t="s">
-        <v>180</v>
       </c>
       <c r="Q1" t="s">
         <v>5</v>
@@ -1094,10 +1094,10 @@
         <v>170</v>
       </c>
       <c r="K2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="N2">
         <v>12</v>
@@ -1106,7 +1106,7 @@
         <v>42</v>
       </c>
       <c r="P2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q2" t="s">
         <v>68</v>
@@ -1141,13 +1141,13 @@
         <v>171</v>
       </c>
       <c r="K3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N3">
         <v>3</v>
@@ -1156,7 +1156,7 @@
         <v>21</v>
       </c>
       <c r="P3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -1185,13 +1185,13 @@
         <v>171</v>
       </c>
       <c r="K4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L4" t="s">
+        <v>189</v>
+      </c>
+      <c r="M4" t="s">
         <v>192</v>
-      </c>
-      <c r="M4" t="s">
-        <v>195</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -1200,7 +1200,7 @@
         <v>36</v>
       </c>
       <c r="P4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1229,13 +1229,13 @@
         <v>171</v>
       </c>
       <c r="K5" t="s">
+        <v>191</v>
+      </c>
+      <c r="L5" t="s">
+        <v>189</v>
+      </c>
+      <c r="M5" t="s">
         <v>194</v>
-      </c>
-      <c r="L5" t="s">
-        <v>192</v>
-      </c>
-      <c r="M5" t="s">
-        <v>197</v>
       </c>
       <c r="N5">
         <v>13</v>
@@ -1244,7 +1244,7 @@
         <v>28</v>
       </c>
       <c r="P5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
@@ -1273,13 +1273,13 @@
         <v>171</v>
       </c>
       <c r="K6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N6">
         <v>12</v>
@@ -1288,7 +1288,7 @@
         <v>33</v>
       </c>
       <c r="P6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -1317,13 +1317,13 @@
         <v>171</v>
       </c>
       <c r="K7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N7">
         <v>5</v>
@@ -1332,7 +1332,7 @@
         <v>40</v>
       </c>
       <c r="P7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -1361,13 +1361,13 @@
         <v>171</v>
       </c>
       <c r="K8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N8">
         <v>5</v>
@@ -1376,7 +1376,7 @@
         <v>25</v>
       </c>
       <c r="P8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1405,13 +1405,13 @@
         <v>171</v>
       </c>
       <c r="K9" t="s">
+        <v>191</v>
+      </c>
+      <c r="L9" t="s">
+        <v>190</v>
+      </c>
+      <c r="M9" t="s">
         <v>194</v>
-      </c>
-      <c r="L9" t="s">
-        <v>193</v>
-      </c>
-      <c r="M9" t="s">
-        <v>197</v>
       </c>
       <c r="N9">
         <v>52</v>
@@ -1420,7 +1420,7 @@
         <v>57</v>
       </c>
       <c r="P9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q9" t="s">
         <v>68</v>
@@ -1455,13 +1455,13 @@
         <v>171</v>
       </c>
       <c r="K10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1470,7 +1470,7 @@
         <v>54</v>
       </c>
       <c r="P10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q10" t="s">
         <v>68</v>
@@ -1505,16 +1505,16 @@
         <v>171</v>
       </c>
       <c r="K11" t="s">
+        <v>191</v>
+      </c>
+      <c r="L11" t="s">
+        <v>190</v>
+      </c>
+      <c r="M11" t="s">
         <v>194</v>
       </c>
-      <c r="L11" t="s">
-        <v>193</v>
-      </c>
-      <c r="M11" t="s">
-        <v>197</v>
-      </c>
       <c r="P11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -1540,13 +1540,13 @@
         <v>171</v>
       </c>
       <c r="K12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L12" t="s">
+        <v>189</v>
+      </c>
+      <c r="M12" t="s">
         <v>192</v>
-      </c>
-      <c r="M12" t="s">
-        <v>195</v>
       </c>
       <c r="N12">
         <v>34</v>
@@ -1555,7 +1555,7 @@
         <v>56</v>
       </c>
       <c r="P12" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q12" t="s">
         <v>68</v>
@@ -1590,13 +1590,13 @@
         <v>171</v>
       </c>
       <c r="K13" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L13" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M13" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N13">
         <v>8</v>
@@ -1605,7 +1605,7 @@
         <v>29</v>
       </c>
       <c r="P13" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
@@ -1631,7 +1631,7 @@
         <v>171</v>
       </c>
       <c r="L14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
@@ -1660,13 +1660,13 @@
         <v>171</v>
       </c>
       <c r="K15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L15" t="s">
+        <v>190</v>
+      </c>
+      <c r="M15" t="s">
         <v>194</v>
-      </c>
-      <c r="L15" t="s">
-        <v>193</v>
-      </c>
-      <c r="M15" t="s">
-        <v>197</v>
       </c>
       <c r="N15">
         <v>17</v>
@@ -1675,7 +1675,7 @@
         <v>25</v>
       </c>
       <c r="P15" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q15" t="s">
         <v>68</v>
@@ -1710,13 +1710,13 @@
         <v>171</v>
       </c>
       <c r="K16" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L16" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N16">
         <v>19</v>
@@ -1725,7 +1725,7 @@
         <v>24</v>
       </c>
       <c r="P16" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q16" t="s">
         <v>68</v>
@@ -1757,13 +1757,13 @@
         <v>171</v>
       </c>
       <c r="K17" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L17" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M17" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -1772,7 +1772,7 @@
         <v>35</v>
       </c>
       <c r="P17" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q17" t="s">
         <v>68</v>
@@ -1847,13 +1847,13 @@
         <v>171</v>
       </c>
       <c r="K20" t="s">
+        <v>191</v>
+      </c>
+      <c r="L20" t="s">
+        <v>189</v>
+      </c>
+      <c r="M20" t="s">
         <v>194</v>
-      </c>
-      <c r="L20" t="s">
-        <v>192</v>
-      </c>
-      <c r="M20" t="s">
-        <v>197</v>
       </c>
       <c r="N20">
         <v>20</v>
@@ -1862,7 +1862,7 @@
         <v>48</v>
       </c>
       <c r="P20" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q20" t="s">
         <v>68</v>
@@ -1894,7 +1894,7 @@
         <v>171</v>
       </c>
       <c r="L21" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
@@ -1960,7 +1960,7 @@
         <v>171</v>
       </c>
       <c r="L24" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
@@ -1989,13 +1989,13 @@
         <v>171</v>
       </c>
       <c r="K25" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L25" t="s">
+        <v>189</v>
+      </c>
+      <c r="M25" t="s">
         <v>192</v>
-      </c>
-      <c r="M25" t="s">
-        <v>195</v>
       </c>
       <c r="N25">
         <v>27</v>
@@ -2004,7 +2004,7 @@
         <v>39</v>
       </c>
       <c r="P25" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q25" t="s">
         <v>68</v>
@@ -2039,13 +2039,13 @@
         <v>171</v>
       </c>
       <c r="K26" t="s">
+        <v>191</v>
+      </c>
+      <c r="L26" t="s">
+        <v>190</v>
+      </c>
+      <c r="M26" t="s">
         <v>194</v>
-      </c>
-      <c r="L26" t="s">
-        <v>193</v>
-      </c>
-      <c r="M26" t="s">
-        <v>197</v>
       </c>
       <c r="N26">
         <v>24</v>
@@ -2054,7 +2054,7 @@
         <v>45</v>
       </c>
       <c r="P26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q26" t="s">
         <v>68</v>
@@ -2089,13 +2089,13 @@
         <v>171</v>
       </c>
       <c r="K27" t="s">
+        <v>191</v>
+      </c>
+      <c r="L27" t="s">
+        <v>189</v>
+      </c>
+      <c r="M27" t="s">
         <v>194</v>
-      </c>
-      <c r="L27" t="s">
-        <v>192</v>
-      </c>
-      <c r="M27" t="s">
-        <v>197</v>
       </c>
       <c r="N27">
         <v>5</v>
@@ -2104,7 +2104,7 @@
         <v>36</v>
       </c>
       <c r="P27" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q27" t="s">
         <v>68</v>
@@ -2136,13 +2136,13 @@
         <v>171</v>
       </c>
       <c r="K28" t="s">
+        <v>191</v>
+      </c>
+      <c r="L28" t="s">
+        <v>189</v>
+      </c>
+      <c r="M28" t="s">
         <v>194</v>
-      </c>
-      <c r="L28" t="s">
-        <v>192</v>
-      </c>
-      <c r="M28" t="s">
-        <v>197</v>
       </c>
       <c r="N28">
         <v>28</v>
@@ -2151,7 +2151,7 @@
         <v>40</v>
       </c>
       <c r="P28" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q28" t="s">
         <v>68</v>
@@ -2186,13 +2186,13 @@
         <v>170</v>
       </c>
       <c r="K29" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L29" t="s">
+        <v>189</v>
+      </c>
+      <c r="M29" t="s">
         <v>192</v>
-      </c>
-      <c r="M29" t="s">
-        <v>195</v>
       </c>
       <c r="N29">
         <v>0</v>
@@ -2201,7 +2201,7 @@
         <v>21</v>
       </c>
       <c r="P29" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q29" t="s">
         <v>68</v>
@@ -2285,13 +2285,13 @@
         <v>170</v>
       </c>
       <c r="K32" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L32" t="s">
+        <v>189</v>
+      </c>
+      <c r="M32" t="s">
         <v>192</v>
-      </c>
-      <c r="M32" t="s">
-        <v>195</v>
       </c>
       <c r="N32">
         <v>42</v>
@@ -2300,7 +2300,7 @@
         <v>59</v>
       </c>
       <c r="P32" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q32" t="s">
         <v>68</v>
@@ -2335,13 +2335,13 @@
         <v>170</v>
       </c>
       <c r="K33" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L33" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M33" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N33">
         <v>12</v>
@@ -2350,7 +2350,7 @@
         <v>39</v>
       </c>
       <c r="P33" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q33" t="s">
         <v>68</v>
@@ -2379,7 +2379,7 @@
         <v>168</v>
       </c>
       <c r="L34" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
@@ -2454,13 +2454,13 @@
         <v>171</v>
       </c>
       <c r="K37" t="s">
+        <v>191</v>
+      </c>
+      <c r="L37" t="s">
+        <v>190</v>
+      </c>
+      <c r="M37" t="s">
         <v>194</v>
-      </c>
-      <c r="L37" t="s">
-        <v>193</v>
-      </c>
-      <c r="M37" t="s">
-        <v>197</v>
       </c>
       <c r="N37">
         <v>48</v>
@@ -2469,7 +2469,7 @@
         <v>57</v>
       </c>
       <c r="P37" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q37" t="s">
         <v>68</v>
@@ -2524,7 +2524,7 @@
         <v>170</v>
       </c>
       <c r="L39" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
@@ -2553,13 +2553,13 @@
         <v>170</v>
       </c>
       <c r="K40" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L40" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M40" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N40">
         <v>20</v>
@@ -2568,7 +2568,7 @@
         <v>46</v>
       </c>
       <c r="P40" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q40" t="s">
         <v>68</v>
@@ -2629,13 +2629,13 @@
         <v>170</v>
       </c>
       <c r="K42" t="s">
+        <v>191</v>
+      </c>
+      <c r="L42" t="s">
+        <v>190</v>
+      </c>
+      <c r="M42" t="s">
         <v>194</v>
-      </c>
-      <c r="L42" t="s">
-        <v>193</v>
-      </c>
-      <c r="M42" t="s">
-        <v>197</v>
       </c>
       <c r="N42">
         <v>47</v>
@@ -2644,7 +2644,7 @@
         <v>52</v>
       </c>
       <c r="P42" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q42" t="s">
         <v>68</v>
@@ -2702,13 +2702,13 @@
         <v>170</v>
       </c>
       <c r="K44" t="s">
+        <v>191</v>
+      </c>
+      <c r="L44" t="s">
+        <v>189</v>
+      </c>
+      <c r="M44" t="s">
         <v>194</v>
-      </c>
-      <c r="L44" t="s">
-        <v>192</v>
-      </c>
-      <c r="M44" t="s">
-        <v>197</v>
       </c>
       <c r="N44">
         <v>34</v>
@@ -2717,7 +2717,7 @@
         <v>37</v>
       </c>
       <c r="P44" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q44" t="s">
         <v>68</v>
@@ -2749,7 +2749,7 @@
         <v>170</v>
       </c>
       <c r="L45" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
@@ -2778,13 +2778,13 @@
         <v>170</v>
       </c>
       <c r="K46" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L46" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M46" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N46">
         <v>29</v>
@@ -2793,7 +2793,7 @@
         <v>38</v>
       </c>
       <c r="P46" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q46" t="s">
         <v>68</v>
@@ -2828,13 +2828,13 @@
         <v>170</v>
       </c>
       <c r="K47" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L47" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M47" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N47">
         <v>0</v>
@@ -2843,7 +2843,7 @@
         <v>20</v>
       </c>
       <c r="P47" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q47" t="s">
         <v>68</v>
@@ -2878,13 +2878,13 @@
         <v>170</v>
       </c>
       <c r="K48" t="s">
+        <v>191</v>
+      </c>
+      <c r="L48" t="s">
+        <v>190</v>
+      </c>
+      <c r="M48" t="s">
         <v>194</v>
-      </c>
-      <c r="L48" t="s">
-        <v>193</v>
-      </c>
-      <c r="M48" t="s">
-        <v>197</v>
       </c>
       <c r="N48">
         <v>26</v>
@@ -2893,7 +2893,7 @@
         <v>47</v>
       </c>
       <c r="P48" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q48" t="s">
         <v>68</v>
@@ -2928,13 +2928,13 @@
         <v>170</v>
       </c>
       <c r="K49" t="s">
+        <v>191</v>
+      </c>
+      <c r="L49" t="s">
+        <v>189</v>
+      </c>
+      <c r="M49" t="s">
         <v>194</v>
-      </c>
-      <c r="L49" t="s">
-        <v>192</v>
-      </c>
-      <c r="M49" t="s">
-        <v>197</v>
       </c>
       <c r="N49">
         <v>14</v>
@@ -2943,7 +2943,7 @@
         <v>30</v>
       </c>
       <c r="P49" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q49" t="s">
         <v>68</v>
@@ -3001,7 +3001,7 @@
         <v>170</v>
       </c>
       <c r="L51" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.2">
@@ -3111,13 +3111,13 @@
         <v>170</v>
       </c>
       <c r="K55" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L55" t="s">
+        <v>189</v>
+      </c>
+      <c r="M55" t="s">
         <v>192</v>
-      </c>
-      <c r="M55" t="s">
-        <v>195</v>
       </c>
       <c r="N55">
         <v>4</v>
@@ -3126,7 +3126,7 @@
         <v>17</v>
       </c>
       <c r="P55" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q55" t="s">
         <v>68</v>
@@ -3161,16 +3161,16 @@
         <v>170</v>
       </c>
       <c r="K56" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L56" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M56" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="P56" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q56" t="s">
         <v>68</v>
@@ -3199,7 +3199,7 @@
         <v>170</v>
       </c>
       <c r="L57" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.2">
@@ -3228,13 +3228,13 @@
         <v>170</v>
       </c>
       <c r="K58" t="s">
+        <v>191</v>
+      </c>
+      <c r="L58" t="s">
+        <v>190</v>
+      </c>
+      <c r="M58" t="s">
         <v>194</v>
-      </c>
-      <c r="L58" t="s">
-        <v>193</v>
-      </c>
-      <c r="M58" t="s">
-        <v>197</v>
       </c>
       <c r="N58">
         <v>16</v>
@@ -3243,7 +3243,7 @@
         <v>25</v>
       </c>
       <c r="P58" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q58" t="s">
         <v>68</v>
@@ -3278,13 +3278,13 @@
         <v>170</v>
       </c>
       <c r="K59" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L59" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M59" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N59">
         <v>7</v>
@@ -3293,7 +3293,7 @@
         <v>32</v>
       </c>
       <c r="P59" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q59" t="s">
         <v>68</v>
@@ -3380,13 +3380,13 @@
         <v>170</v>
       </c>
       <c r="K62" t="s">
+        <v>191</v>
+      </c>
+      <c r="L62" t="s">
+        <v>190</v>
+      </c>
+      <c r="M62" t="s">
         <v>194</v>
-      </c>
-      <c r="L62" t="s">
-        <v>193</v>
-      </c>
-      <c r="M62" t="s">
-        <v>197</v>
       </c>
       <c r="N62">
         <v>32</v>
@@ -3395,7 +3395,7 @@
         <v>42</v>
       </c>
       <c r="P62" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q62" t="s">
         <v>68</v>
@@ -3430,13 +3430,13 @@
         <v>170</v>
       </c>
       <c r="K63" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L63" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M63" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N63">
         <v>14</v>
@@ -3445,7 +3445,7 @@
         <v>34</v>
       </c>
       <c r="P63" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q63" t="s">
         <v>68</v>
@@ -3480,13 +3480,13 @@
         <v>170</v>
       </c>
       <c r="K64" t="s">
+        <v>191</v>
+      </c>
+      <c r="L64" t="s">
+        <v>189</v>
+      </c>
+      <c r="M64" t="s">
         <v>194</v>
-      </c>
-      <c r="L64" t="s">
-        <v>192</v>
-      </c>
-      <c r="M64" t="s">
-        <v>197</v>
       </c>
       <c r="N64">
         <v>12</v>
@@ -3495,7 +3495,7 @@
         <v>21</v>
       </c>
       <c r="P64" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q64" t="s">
         <v>68</v>
@@ -3556,13 +3556,13 @@
         <v>170</v>
       </c>
       <c r="K66" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L66" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M66" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N66">
         <v>3</v>
@@ -3571,7 +3571,7 @@
         <v>21</v>
       </c>
       <c r="P66" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.2">
@@ -3600,13 +3600,13 @@
         <v>170</v>
       </c>
       <c r="K67" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L67" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M67" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N67">
         <v>6</v>
@@ -3615,7 +3615,7 @@
         <v>50</v>
       </c>
       <c r="P67" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.2">
@@ -3644,13 +3644,13 @@
         <v>170</v>
       </c>
       <c r="K68" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L68" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M68" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N68">
         <v>2</v>
@@ -3659,7 +3659,7 @@
         <v>28</v>
       </c>
       <c r="P68" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.2">
@@ -3688,13 +3688,13 @@
         <v>170</v>
       </c>
       <c r="K69" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L69" t="s">
+        <v>189</v>
+      </c>
+      <c r="M69" t="s">
         <v>192</v>
-      </c>
-      <c r="M69" t="s">
-        <v>195</v>
       </c>
       <c r="N69">
         <v>12</v>
@@ -3703,7 +3703,7 @@
         <v>24</v>
       </c>
       <c r="P69" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.2">
@@ -3732,13 +3732,13 @@
         <v>170</v>
       </c>
       <c r="K70" t="s">
+        <v>191</v>
+      </c>
+      <c r="L70" t="s">
+        <v>189</v>
+      </c>
+      <c r="M70" t="s">
         <v>194</v>
-      </c>
-      <c r="L70" t="s">
-        <v>192</v>
-      </c>
-      <c r="M70" t="s">
-        <v>197</v>
       </c>
       <c r="N70">
         <v>5</v>
@@ -3747,7 +3747,7 @@
         <v>42</v>
       </c>
       <c r="P70" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.2">
@@ -3776,13 +3776,13 @@
         <v>170</v>
       </c>
       <c r="K71" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L71" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M71" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N71">
         <v>13</v>
@@ -3791,7 +3791,7 @@
         <v>20</v>
       </c>
       <c r="P71" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.2">
@@ -3820,13 +3820,13 @@
         <v>170</v>
       </c>
       <c r="K72" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L72" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M72" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N72">
         <v>2</v>
@@ -3835,7 +3835,7 @@
         <v>28</v>
       </c>
       <c r="P72" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.2">
@@ -3864,13 +3864,13 @@
         <v>170</v>
       </c>
       <c r="K73" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L73" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M73" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N73">
         <v>16</v>
@@ -3879,7 +3879,7 @@
         <v>31</v>
       </c>
       <c r="P73" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.2">
@@ -3905,7 +3905,7 @@
         <v>170</v>
       </c>
       <c r="L74" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.2">
@@ -3934,13 +3934,13 @@
         <v>170</v>
       </c>
       <c r="K75" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L75" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M75" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N75">
         <v>9</v>
@@ -3949,7 +3949,7 @@
         <v>38</v>
       </c>
       <c r="P75" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.2">
@@ -3998,13 +3998,13 @@
         <v>170</v>
       </c>
       <c r="K77" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L77" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M77" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N77">
         <v>9</v>
@@ -4013,7 +4013,7 @@
         <v>24</v>
       </c>
       <c r="P77" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.2">
@@ -4036,13 +4036,13 @@
         <v>170</v>
       </c>
       <c r="K78" t="s">
+        <v>191</v>
+      </c>
+      <c r="L78" t="s">
+        <v>190</v>
+      </c>
+      <c r="M78" t="s">
         <v>194</v>
-      </c>
-      <c r="L78" t="s">
-        <v>193</v>
-      </c>
-      <c r="M78" t="s">
-        <v>197</v>
       </c>
       <c r="N78">
         <v>12</v>
@@ -4051,15 +4051,15 @@
         <v>25</v>
       </c>
       <c r="P78" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B79" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C79" t="s">
         <v>68</v>
@@ -4080,10 +4080,10 @@
         <v>171</v>
       </c>
       <c r="K79" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L79" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="N79">
         <v>23</v>
@@ -4092,15 +4092,15 @@
         <v>37</v>
       </c>
       <c r="P79" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B80" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C80" t="s">
         <v>68</v>
@@ -4121,10 +4121,10 @@
         <v>171</v>
       </c>
       <c r="K80" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L80" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="N80">
         <v>5</v>
@@ -4133,15 +4133,15 @@
         <v>36</v>
       </c>
       <c r="P80" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B81" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C81" t="s">
         <v>68</v>
@@ -4162,24 +4162,24 @@
         <v>171</v>
       </c>
       <c r="K81" t="s">
+        <v>191</v>
+      </c>
+      <c r="L81" t="s">
+        <v>189</v>
+      </c>
+      <c r="M81" t="s">
         <v>194</v>
       </c>
-      <c r="L81" t="s">
-        <v>192</v>
-      </c>
-      <c r="M81" t="s">
-        <v>197</v>
-      </c>
       <c r="P81" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B82" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C82" t="s">
         <v>68</v>
@@ -4200,13 +4200,13 @@
         <v>171</v>
       </c>
       <c r="K82" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L82" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M82" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N82">
         <v>31</v>
@@ -4215,15 +4215,15 @@
         <v>33</v>
       </c>
       <c r="P82" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B83" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C83" t="s">
         <v>68</v>
@@ -4244,10 +4244,10 @@
         <v>171</v>
       </c>
       <c r="K83" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L83" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="N83">
         <v>5</v>
@@ -4256,15 +4256,15 @@
         <v>10</v>
       </c>
       <c r="P83" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>183</v>
+      </c>
+      <c r="B84" t="s">
         <v>186</v>
-      </c>
-      <c r="B84" t="s">
-        <v>189</v>
       </c>
       <c r="C84" t="s">
         <v>68</v>
@@ -4285,24 +4285,24 @@
         <v>171</v>
       </c>
       <c r="K84" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L84" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M84" t="s">
+        <v>192</v>
+      </c>
+      <c r="P84" t="s">
         <v>195</v>
-      </c>
-      <c r="P84" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B85" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C85" t="s">
         <v>68</v>
@@ -4323,10 +4323,10 @@
         <v>171</v>
       </c>
       <c r="L85" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M85" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N85">
         <v>4</v>
@@ -4335,15 +4335,15 @@
         <v>5</v>
       </c>
       <c r="P85" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B86" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C86" t="s">
         <v>68</v>
@@ -4364,16 +4364,16 @@
         <v>171</v>
       </c>
       <c r="K86" t="s">
+        <v>191</v>
+      </c>
+      <c r="L86" t="s">
+        <v>189</v>
+      </c>
+      <c r="M86" t="s">
         <v>194</v>
       </c>
-      <c r="L86" t="s">
-        <v>192</v>
-      </c>
-      <c r="M86" t="s">
-        <v>197</v>
-      </c>
       <c r="P86" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HUP082 and lobar data
</commit_message>
<xml_diff>
--- a/data/atlas_project_metadata.xlsx
+++ b/data/atlas_project_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbernabei/Documents/PhD_Research/atlas_project/iEEG_atlas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21323ED-AF3F-9147-AFDF-B042DE7D1766}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A2D4E7-76F4-2A4F-BB54-84F3D66A0492}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16360" yWindow="2120" windowWidth="25260" windowHeight="17720" xr2:uid="{55386E59-C2B1-FE47-8A03-2662CFD6A014}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="205">
   <si>
     <t>Patient</t>
   </si>
@@ -631,6 +631,15 @@
   </si>
   <si>
     <t>Age_surgery</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>MTL</t>
+  </si>
+  <si>
+    <t>MFL</t>
   </si>
 </sst>
 </file>
@@ -984,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEE15CE-15A7-E440-8B77-868E4F33ECBC}">
   <dimension ref="A1:S86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
+      <selection activeCell="K84" sqref="K84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1273,7 +1282,7 @@
         <v>171</v>
       </c>
       <c r="K6" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="L6" t="s">
         <v>190</v>
@@ -2285,7 +2294,7 @@
         <v>170</v>
       </c>
       <c r="K32" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="L32" t="s">
         <v>189</v>
@@ -2553,7 +2562,7 @@
         <v>170</v>
       </c>
       <c r="K40" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="L40" t="s">
         <v>190</v>
@@ -2629,7 +2638,7 @@
         <v>170</v>
       </c>
       <c r="K42" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="L42" t="s">
         <v>190</v>
@@ -2702,7 +2711,7 @@
         <v>170</v>
       </c>
       <c r="K44" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="L44" t="s">
         <v>189</v>
@@ -2778,7 +2787,7 @@
         <v>170</v>
       </c>
       <c r="K46" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="L46" t="s">
         <v>190</v>
@@ -2878,7 +2887,7 @@
         <v>170</v>
       </c>
       <c r="K48" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="L48" t="s">
         <v>190</v>
@@ -2928,7 +2937,7 @@
         <v>170</v>
       </c>
       <c r="K49" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="L49" t="s">
         <v>189</v>
@@ -3161,7 +3170,7 @@
         <v>170</v>
       </c>
       <c r="K56" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="L56" t="s">
         <v>189</v>
@@ -3228,7 +3237,7 @@
         <v>170</v>
       </c>
       <c r="K58" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="L58" t="s">
         <v>190</v>
@@ -3380,7 +3389,7 @@
         <v>170</v>
       </c>
       <c r="K62" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="L62" t="s">
         <v>190</v>
@@ -3430,7 +3439,7 @@
         <v>170</v>
       </c>
       <c r="K63" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="L63" t="s">
         <v>190</v>
@@ -3934,7 +3943,7 @@
         <v>170</v>
       </c>
       <c r="K75" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="L75" t="s">
         <v>190</v>
@@ -4036,7 +4045,7 @@
         <v>170</v>
       </c>
       <c r="K78" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="L78" t="s">
         <v>190</v>
@@ -4321,6 +4330,9 @@
       </c>
       <c r="H85" t="s">
         <v>171</v>
+      </c>
+      <c r="K85" t="s">
+        <v>202</v>
       </c>
       <c r="L85" t="s">
         <v>190</v>

</xml_diff>

<commit_message>
added data and testing bilateral hypotheses
</commit_message>
<xml_diff>
--- a/data/atlas_project_metadata.xlsx
+++ b/data/atlas_project_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbernabei/Documents/PhD_Research/atlas_project/iEEG_atlas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A2D4E7-76F4-2A4F-BB54-84F3D66A0492}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF63A1BF-DBB8-D84C-8BCA-507FE5056F17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16360" yWindow="2120" windowWidth="25260" windowHeight="17720" xr2:uid="{55386E59-C2B1-FE47-8A03-2662CFD6A014}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="205">
   <si>
     <t>Patient</t>
   </si>
@@ -993,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEE15CE-15A7-E440-8B77-868E4F33ECBC}">
   <dimension ref="A1:S86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
-      <selection activeCell="K84" sqref="K84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1536,6 +1536,9 @@
       <c r="C12" t="s">
         <v>68</v>
       </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
       <c r="E12" t="s">
         <v>68</v>
       </c>
@@ -1956,6 +1959,9 @@
       <c r="C24" t="s">
         <v>68</v>
       </c>
+      <c r="D24" t="s">
+        <v>68</v>
+      </c>
       <c r="E24" t="s">
         <v>168</v>
       </c>
@@ -2520,6 +2526,9 @@
       <c r="C39" t="s">
         <v>68</v>
       </c>
+      <c r="D39" t="s">
+        <v>68</v>
+      </c>
       <c r="E39" t="s">
         <v>168</v>
       </c>
@@ -2745,6 +2754,9 @@
       <c r="C45" t="s">
         <v>68</v>
       </c>
+      <c r="D45" t="s">
+        <v>68</v>
+      </c>
       <c r="E45" t="s">
         <v>168</v>
       </c>
@@ -2997,6 +3009,9 @@
       <c r="C51" t="s">
         <v>68</v>
       </c>
+      <c r="D51" t="s">
+        <v>68</v>
+      </c>
       <c r="E51" t="s">
         <v>168</v>
       </c>
@@ -3899,6 +3914,9 @@
         <v>117</v>
       </c>
       <c r="C74" t="s">
+        <v>68</v>
+      </c>
+      <c r="D74" t="s">
         <v>68</v>
       </c>
       <c r="E74" t="s">

</xml_diff>

<commit_message>
writing distance function things
</commit_message>
<xml_diff>
--- a/data/atlas_project_metadata.xlsx
+++ b/data/atlas_project_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbernabei/Documents/PhD_Research/atlas_project/iEEG_atlas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB76763-57B0-8042-8260-FD4F8725CA1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABB4270-52B0-CD42-A046-E1F6ECB90241}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7940" yWindow="760" windowWidth="25260" windowHeight="17720" xr2:uid="{55386E59-C2B1-FE47-8A03-2662CFD6A014}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="224">
   <si>
     <t>Patient</t>
   </si>
@@ -682,6 +682,21 @@
   </si>
   <si>
     <t>L_Insular</t>
+  </si>
+  <si>
+    <t>Prior_surgery</t>
+  </si>
+  <si>
+    <t>PET_lesion</t>
+  </si>
+  <si>
+    <t>Generalized_sz</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1033,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEE15CE-15A7-E440-8B77-868E4F33ECBC}">
-  <dimension ref="A1:S86"/>
+  <dimension ref="A1:V86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="K72" sqref="K72:L72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q79" sqref="Q79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1060,7 +1075,7 @@
     <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1110,16 +1125,25 @@
         <v>175</v>
       </c>
       <c r="Q1" t="s">
+        <v>219</v>
+      </c>
+      <c r="R1" t="s">
+        <v>220</v>
+      </c>
+      <c r="S1" t="s">
+        <v>221</v>
+      </c>
+      <c r="T1" t="s">
         <v>5</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>4</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1160,13 +1184,19 @@
         <v>193</v>
       </c>
       <c r="Q2" t="s">
-        <v>68</v>
+        <v>222</v>
       </c>
       <c r="S2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="T2" t="s">
+        <v>68</v>
+      </c>
+      <c r="V2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1209,8 +1239,11 @@
       <c r="P3" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1253,8 +1286,11 @@
       <c r="P4" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1297,8 +1333,11 @@
       <c r="P5" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1341,8 +1380,11 @@
       <c r="P6" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1385,8 +1427,11 @@
       <c r="P7" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1429,8 +1474,11 @@
       <c r="P8" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1473,14 +1521,17 @@
       <c r="P9" t="s">
         <v>193</v>
       </c>
-      <c r="Q9" t="s">
-        <v>68</v>
-      </c>
       <c r="S9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="T9" t="s">
+        <v>68</v>
+      </c>
+      <c r="V9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1523,14 +1574,17 @@
       <c r="P10" t="s">
         <v>191</v>
       </c>
-      <c r="Q10" t="s">
-        <v>68</v>
-      </c>
       <c r="S10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="T10" t="s">
+        <v>68</v>
+      </c>
+      <c r="V10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1567,8 +1621,11 @@
       <c r="P11" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1611,14 +1668,17 @@
       <c r="P12" t="s">
         <v>193</v>
       </c>
-      <c r="Q12" t="s">
-        <v>68</v>
-      </c>
       <c r="S12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="T12" t="s">
+        <v>68</v>
+      </c>
+      <c r="V12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -1661,8 +1721,11 @@
       <c r="P13" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -1688,7 +1751,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1731,14 +1794,17 @@
       <c r="P15" t="s">
         <v>193</v>
       </c>
-      <c r="Q15" t="s">
-        <v>68</v>
-      </c>
       <c r="S15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="T15" t="s">
+        <v>68</v>
+      </c>
+      <c r="V15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1781,11 +1847,14 @@
       <c r="P16" t="s">
         <v>191</v>
       </c>
-      <c r="Q16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S16" t="s">
+        <v>223</v>
+      </c>
+      <c r="T16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1828,14 +1897,17 @@
       <c r="P17" t="s">
         <v>193</v>
       </c>
-      <c r="Q17" t="s">
-        <v>68</v>
-      </c>
       <c r="S17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="T17" t="s">
+        <v>68</v>
+      </c>
+      <c r="V17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -1855,7 +1927,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -1875,7 +1947,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1918,14 +1990,17 @@
       <c r="P20" t="s">
         <v>193</v>
       </c>
-      <c r="Q20" t="s">
-        <v>68</v>
-      </c>
       <c r="S20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="T20" t="s">
+        <v>68</v>
+      </c>
+      <c r="V20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -1951,7 +2026,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -1971,7 +2046,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -1991,7 +2066,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2020,7 +2095,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -2063,14 +2138,17 @@
       <c r="P25" t="s">
         <v>191</v>
       </c>
-      <c r="Q25" t="s">
-        <v>68</v>
-      </c>
       <c r="S25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="T25" t="s">
+        <v>68</v>
+      </c>
+      <c r="V25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -2113,14 +2191,17 @@
       <c r="P26" t="s">
         <v>193</v>
       </c>
-      <c r="Q26" t="s">
-        <v>68</v>
-      </c>
       <c r="S26" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="T26" t="s">
+        <v>68</v>
+      </c>
+      <c r="V26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -2163,11 +2244,14 @@
       <c r="P27" t="s">
         <v>191</v>
       </c>
-      <c r="Q27" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S27" t="s">
+        <v>222</v>
+      </c>
+      <c r="T27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2210,14 +2294,17 @@
       <c r="P28" t="s">
         <v>193</v>
       </c>
-      <c r="Q28" t="s">
-        <v>68</v>
-      </c>
       <c r="S28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="T28" t="s">
+        <v>68</v>
+      </c>
+      <c r="V28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2261,13 +2348,16 @@
         <v>193</v>
       </c>
       <c r="Q29" t="s">
-        <v>68</v>
-      </c>
-      <c r="S29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="T29" t="s">
+        <v>68</v>
+      </c>
+      <c r="V29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -2287,7 +2377,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -2309,14 +2399,14 @@
       <c r="H31" t="s">
         <v>171</v>
       </c>
-      <c r="Q31" t="s">
-        <v>68</v>
-      </c>
-      <c r="S31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T31" t="s">
+        <v>68</v>
+      </c>
+      <c r="V31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -2366,13 +2456,19 @@
         <v>193</v>
       </c>
       <c r="Q32" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
       <c r="S32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="T32" t="s">
+        <v>68</v>
+      </c>
+      <c r="V32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -2422,13 +2518,19 @@
         <v>191</v>
       </c>
       <c r="Q33" t="s">
-        <v>68</v>
+        <v>222</v>
       </c>
       <c r="S33" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="T33" t="s">
+        <v>68</v>
+      </c>
+      <c r="V33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -2451,7 +2553,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -2470,11 +2572,11 @@
       <c r="H35" t="s">
         <v>171</v>
       </c>
-      <c r="Q35" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -2490,14 +2592,14 @@
       <c r="H36" t="s">
         <v>171</v>
       </c>
-      <c r="Q36" t="s">
-        <v>68</v>
-      </c>
-      <c r="S36" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T36" t="s">
+        <v>68</v>
+      </c>
+      <c r="V36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -2540,14 +2642,14 @@
       <c r="P37" t="s">
         <v>191</v>
       </c>
-      <c r="Q37" t="s">
-        <v>68</v>
-      </c>
-      <c r="S37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T37" t="s">
+        <v>68</v>
+      </c>
+      <c r="V37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -2566,11 +2668,11 @@
       <c r="H38" t="s">
         <v>171</v>
       </c>
-      <c r="Q38" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T38" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -2599,7 +2701,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -2649,13 +2751,19 @@
         <v>193</v>
       </c>
       <c r="Q40" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
       <c r="S40" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="T40" t="s">
+        <v>68</v>
+      </c>
+      <c r="V40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -2674,14 +2782,14 @@
       <c r="H41" t="s">
         <v>170</v>
       </c>
-      <c r="Q41" t="s">
-        <v>68</v>
-      </c>
-      <c r="S41" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T41" t="s">
+        <v>68</v>
+      </c>
+      <c r="V41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -2725,13 +2833,19 @@
         <v>193</v>
       </c>
       <c r="Q42" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
       <c r="S42" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="T42" t="s">
+        <v>68</v>
+      </c>
+      <c r="V42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -2750,14 +2864,14 @@
       <c r="H43" t="s">
         <v>170</v>
       </c>
-      <c r="Q43" t="s">
-        <v>68</v>
-      </c>
-      <c r="S43" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T43" t="s">
+        <v>68</v>
+      </c>
+      <c r="V43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -2804,13 +2918,19 @@
         <v>191</v>
       </c>
       <c r="Q44" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
       <c r="S44" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="T44" t="s">
+        <v>68</v>
+      </c>
+      <c r="V44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>87</v>
       </c>
@@ -2839,7 +2959,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>38</v>
       </c>
@@ -2889,13 +3009,19 @@
         <v>191</v>
       </c>
       <c r="Q46" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
       <c r="S46" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="T46" t="s">
+        <v>68</v>
+      </c>
+      <c r="V46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -2945,13 +3071,19 @@
         <v>191</v>
       </c>
       <c r="Q47" t="s">
-        <v>68</v>
+        <v>222</v>
       </c>
       <c r="S47" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="T47" t="s">
+        <v>68</v>
+      </c>
+      <c r="V47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -3001,13 +3133,19 @@
         <v>193</v>
       </c>
       <c r="Q48" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
       <c r="S48" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="T48" t="s">
+        <v>68</v>
+      </c>
+      <c r="V48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -3057,13 +3195,19 @@
         <v>191</v>
       </c>
       <c r="Q49" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
       <c r="S49" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="T49" t="s">
+        <v>68</v>
+      </c>
+      <c r="V49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -3082,14 +3226,14 @@
       <c r="H50" t="s">
         <v>170</v>
       </c>
-      <c r="Q50" t="s">
-        <v>68</v>
-      </c>
-      <c r="S50" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T50" t="s">
+        <v>68</v>
+      </c>
+      <c r="V50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -3118,7 +3262,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -3137,14 +3281,14 @@
       <c r="H52" t="s">
         <v>170</v>
       </c>
-      <c r="Q52" t="s">
-        <v>68</v>
-      </c>
-      <c r="S52" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T52" t="s">
+        <v>68</v>
+      </c>
+      <c r="V52" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>45</v>
       </c>
@@ -3163,14 +3307,14 @@
       <c r="H53" t="s">
         <v>170</v>
       </c>
-      <c r="Q53" t="s">
-        <v>68</v>
-      </c>
-      <c r="S53" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T53" t="s">
+        <v>68</v>
+      </c>
+      <c r="V53" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>44</v>
       </c>
@@ -3193,13 +3337,16 @@
         <v>170</v>
       </c>
       <c r="Q54" t="s">
-        <v>68</v>
-      </c>
-      <c r="S54" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="T54" t="s">
+        <v>68</v>
+      </c>
+      <c r="V54" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>46</v>
       </c>
@@ -3249,13 +3396,19 @@
         <v>191</v>
       </c>
       <c r="Q55" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
       <c r="S55" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="T55" t="s">
+        <v>68</v>
+      </c>
+      <c r="V55" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>47</v>
       </c>
@@ -3296,13 +3449,19 @@
         <v>191</v>
       </c>
       <c r="Q56" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
       <c r="S56" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="T56" t="s">
+        <v>68</v>
+      </c>
+      <c r="V56" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>89</v>
       </c>
@@ -3325,7 +3484,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>48</v>
       </c>
@@ -3375,13 +3534,19 @@
         <v>191</v>
       </c>
       <c r="Q58" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
       <c r="S58" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="T58" t="s">
+        <v>68</v>
+      </c>
+      <c r="V58" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>49</v>
       </c>
@@ -3431,13 +3596,19 @@
         <v>191</v>
       </c>
       <c r="Q59" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
       <c r="S59" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="T59" t="s">
+        <v>68</v>
+      </c>
+      <c r="V59" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>50</v>
       </c>
@@ -3456,14 +3627,14 @@
       <c r="H60" t="s">
         <v>170</v>
       </c>
-      <c r="Q60" t="s">
-        <v>68</v>
-      </c>
-      <c r="S60" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T60" t="s">
+        <v>68</v>
+      </c>
+      <c r="V60" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>51</v>
       </c>
@@ -3482,14 +3653,14 @@
       <c r="H61" t="s">
         <v>170</v>
       </c>
-      <c r="Q61" t="s">
-        <v>68</v>
-      </c>
-      <c r="S61" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T61" t="s">
+        <v>68</v>
+      </c>
+      <c r="V61" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>52</v>
       </c>
@@ -3539,13 +3710,19 @@
         <v>193</v>
       </c>
       <c r="Q62" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
       <c r="S62" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="T62" t="s">
+        <v>68</v>
+      </c>
+      <c r="V62" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>53</v>
       </c>
@@ -3595,13 +3772,19 @@
         <v>193</v>
       </c>
       <c r="Q63" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
       <c r="S63" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="T63" t="s">
+        <v>68</v>
+      </c>
+      <c r="V63" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>54</v>
       </c>
@@ -3650,14 +3833,14 @@
       <c r="P64" t="s">
         <v>193</v>
       </c>
-      <c r="Q64" t="s">
-        <v>68</v>
-      </c>
-      <c r="S64" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T64" t="s">
+        <v>68</v>
+      </c>
+      <c r="V64" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -3676,14 +3859,14 @@
       <c r="H65" t="s">
         <v>170</v>
       </c>
-      <c r="Q65" t="s">
-        <v>68</v>
-      </c>
-      <c r="S65" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T65" t="s">
+        <v>68</v>
+      </c>
+      <c r="V65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>56</v>
       </c>
@@ -3732,8 +3915,14 @@
       <c r="P66" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q66" t="s">
+        <v>223</v>
+      </c>
+      <c r="S66" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>57</v>
       </c>
@@ -3782,8 +3971,14 @@
       <c r="P67" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q67" t="s">
+        <v>223</v>
+      </c>
+      <c r="S67" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>58</v>
       </c>
@@ -3832,8 +4027,14 @@
       <c r="P68" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q68" t="s">
+        <v>223</v>
+      </c>
+      <c r="S68" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>59</v>
       </c>
@@ -3882,8 +4083,11 @@
       <c r="P69" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q69" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>60</v>
       </c>
@@ -3932,8 +4136,14 @@
       <c r="P70" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q70" t="s">
+        <v>223</v>
+      </c>
+      <c r="S70" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>61</v>
       </c>
@@ -3976,8 +4186,11 @@
       <c r="P71" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q71" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>62</v>
       </c>
@@ -4020,8 +4233,11 @@
       <c r="P72" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q72" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>63</v>
       </c>
@@ -4070,8 +4286,14 @@
       <c r="P73" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q73" t="s">
+        <v>223</v>
+      </c>
+      <c r="S73" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>90</v>
       </c>
@@ -4100,7 +4322,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>64</v>
       </c>
@@ -4149,8 +4371,14 @@
       <c r="P75" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q75" t="s">
+        <v>223</v>
+      </c>
+      <c r="S75" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>65</v>
       </c>
@@ -4170,7 +4398,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>66</v>
       </c>
@@ -4219,8 +4447,11 @@
       <c r="P77" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q77" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>67</v>
       </c>
@@ -4263,8 +4494,14 @@
       <c r="P78" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q78" t="s">
+        <v>223</v>
+      </c>
+      <c r="S78" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>176</v>
       </c>
@@ -4305,7 +4542,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>177</v>
       </c>

</xml_diff>

<commit_message>
major update to current code
</commit_message>
<xml_diff>
--- a/data/atlas_project_metadata.xlsx
+++ b/data/atlas_project_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbernabei/Documents/PhD_Research/atlas_project/iEEG_atlas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07062504-0A4C-A94E-87D4-6A3984CD9C1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8030506-1485-F149-AF9D-F46D564D1F00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7940" yWindow="760" windowWidth="25260" windowHeight="17720" xr2:uid="{55386E59-C2B1-FE47-8A03-2662CFD6A014}"/>
+    <workbookView xWindow="11620" yWindow="2560" windowWidth="25260" windowHeight="17720" xr2:uid="{55386E59-C2B1-FE47-8A03-2662CFD6A014}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="206">
   <si>
     <t>Patient</t>
   </si>
@@ -273,33 +273,6 @@
     <t>HUP113</t>
   </si>
   <si>
-    <t>HUP084</t>
-  </si>
-  <si>
-    <t>HUP096</t>
-  </si>
-  <si>
-    <t>HUP101</t>
-  </si>
-  <si>
-    <t>HUP119</t>
-  </si>
-  <si>
-    <t>HUP127</t>
-  </si>
-  <si>
-    <t>HUP137</t>
-  </si>
-  <si>
-    <t>HUP143</t>
-  </si>
-  <si>
-    <t>HUP153</t>
-  </si>
-  <si>
-    <t>HUP182</t>
-  </si>
-  <si>
     <t>RID0490</t>
   </si>
   <si>
@@ -378,9 +351,6 @@
     <t>RID0522</t>
   </si>
   <si>
-    <t>RID0502</t>
-  </si>
-  <si>
     <t>RID0230</t>
   </si>
   <si>
@@ -393,36 +363,24 @@
     <t>RID0381</t>
   </si>
   <si>
-    <t>RID0328</t>
-  </si>
-  <si>
     <t>RID0301</t>
   </si>
   <si>
     <t>RID0112</t>
   </si>
   <si>
-    <t>RID0206</t>
-  </si>
-  <si>
     <t>RID0295</t>
   </si>
   <si>
     <t>RID0320</t>
   </si>
   <si>
-    <t>RID0280</t>
-  </si>
-  <si>
     <t>RID0194</t>
   </si>
   <si>
     <t>RID0282</t>
   </si>
   <si>
-    <t>RID0186</t>
-  </si>
-  <si>
     <t>RID0089</t>
   </si>
   <si>
@@ -435,9 +393,6 @@
     <t>RID0193</t>
   </si>
   <si>
-    <t>RID0213</t>
-  </si>
-  <si>
     <t>RID0192</t>
   </si>
   <si>
@@ -462,18 +417,12 @@
     <t>RID0101</t>
   </si>
   <si>
-    <t>RID0102</t>
-  </si>
-  <si>
     <t>RID0032</t>
   </si>
   <si>
     <t>RID0033</t>
   </si>
   <si>
-    <t>RID0030</t>
-  </si>
-  <si>
     <t>RID0051</t>
   </si>
   <si>
@@ -492,9 +441,6 @@
     <t>RID0018</t>
   </si>
   <si>
-    <t>RID0015</t>
-  </si>
-  <si>
     <t>RID0014</t>
   </si>
   <si>
@@ -531,9 +477,6 @@
     <t>patient_data.mat</t>
   </si>
   <si>
-    <t>RNS</t>
-  </si>
-  <si>
     <t>Echobase</t>
   </si>
   <si>
@@ -612,9 +555,6 @@
     <t>Parietal</t>
   </si>
   <si>
-    <t>Bilateral</t>
-  </si>
-  <si>
     <t>Insular</t>
   </si>
   <si>
@@ -697,6 +637,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>no elecs</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -1050,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEE15CE-15A7-E440-8B77-868E4F33ECBC}">
   <dimension ref="A1:V86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1083,10 +1029,10 @@
         <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="D1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -1098,40 +1044,40 @@
         <v>75</v>
       </c>
       <c r="H1" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="I1" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="J1" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="K1" t="s">
         <v>76</v>
       </c>
       <c r="L1" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="M1" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="N1" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="O1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q1" t="s">
         <v>199</v>
       </c>
-      <c r="P1" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>219</v>
-      </c>
       <c r="R1" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="S1" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="T1" t="s">
         <v>5</v>
@@ -1163,16 +1109,16 @@
         <v>69</v>
       </c>
       <c r="G2" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H2" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="K2" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="L2" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="N2">
         <v>12</v>
@@ -1181,13 +1127,13 @@
         <v>42</v>
       </c>
       <c r="P2" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="Q2" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="S2" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="T2" t="s">
         <v>68</v>
@@ -1201,7 +1147,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
         <v>68</v>
@@ -1216,19 +1162,19 @@
         <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H3" t="s">
+        <v>152</v>
+      </c>
+      <c r="K3" t="s">
+        <v>167</v>
+      </c>
+      <c r="L3" t="s">
+        <v>169</v>
+      </c>
+      <c r="M3" t="s">
         <v>171</v>
-      </c>
-      <c r="K3" t="s">
-        <v>186</v>
-      </c>
-      <c r="L3" t="s">
-        <v>188</v>
-      </c>
-      <c r="M3" t="s">
-        <v>190</v>
       </c>
       <c r="N3">
         <v>3</v>
@@ -1237,10 +1183,10 @@
         <v>21</v>
       </c>
       <c r="P3" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="S3" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
@@ -1248,7 +1194,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
         <v>68</v>
@@ -1263,19 +1209,19 @@
         <v>70</v>
       </c>
       <c r="G4" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H4" t="s">
+        <v>152</v>
+      </c>
+      <c r="K4" t="s">
+        <v>170</v>
+      </c>
+      <c r="L4" t="s">
+        <v>168</v>
+      </c>
+      <c r="M4" t="s">
         <v>171</v>
-      </c>
-      <c r="K4" t="s">
-        <v>189</v>
-      </c>
-      <c r="L4" t="s">
-        <v>187</v>
-      </c>
-      <c r="M4" t="s">
-        <v>190</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -1284,10 +1230,10 @@
         <v>36</v>
       </c>
       <c r="P4" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="S4" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -1295,7 +1241,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
         <v>68</v>
@@ -1310,19 +1256,19 @@
         <v>71</v>
       </c>
       <c r="G5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H5" t="s">
+        <v>152</v>
+      </c>
+      <c r="K5" t="s">
+        <v>170</v>
+      </c>
+      <c r="L5" t="s">
+        <v>168</v>
+      </c>
+      <c r="M5" t="s">
         <v>173</v>
-      </c>
-      <c r="H5" t="s">
-        <v>171</v>
-      </c>
-      <c r="K5" t="s">
-        <v>189</v>
-      </c>
-      <c r="L5" t="s">
-        <v>187</v>
-      </c>
-      <c r="M5" t="s">
-        <v>192</v>
       </c>
       <c r="N5">
         <v>13</v>
@@ -1331,10 +1277,10 @@
         <v>28</v>
       </c>
       <c r="P5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="S5" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
@@ -1342,7 +1288,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="C6" t="s">
         <v>68</v>
@@ -1357,19 +1303,19 @@
         <v>70</v>
       </c>
       <c r="G6" t="s">
+        <v>154</v>
+      </c>
+      <c r="H6" t="s">
+        <v>152</v>
+      </c>
+      <c r="K6" t="s">
+        <v>180</v>
+      </c>
+      <c r="L6" t="s">
+        <v>169</v>
+      </c>
+      <c r="M6" t="s">
         <v>173</v>
-      </c>
-      <c r="H6" t="s">
-        <v>171</v>
-      </c>
-      <c r="K6" t="s">
-        <v>200</v>
-      </c>
-      <c r="L6" t="s">
-        <v>188</v>
-      </c>
-      <c r="M6" t="s">
-        <v>192</v>
       </c>
       <c r="N6">
         <v>12</v>
@@ -1378,10 +1324,10 @@
         <v>33</v>
       </c>
       <c r="P6" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="S6" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
@@ -1389,7 +1335,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="C7" t="s">
         <v>68</v>
@@ -1404,19 +1350,19 @@
         <v>70</v>
       </c>
       <c r="G7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H7" t="s">
+        <v>152</v>
+      </c>
+      <c r="K7" t="s">
+        <v>167</v>
+      </c>
+      <c r="L7" t="s">
+        <v>168</v>
+      </c>
+      <c r="M7" t="s">
         <v>173</v>
-      </c>
-      <c r="H7" t="s">
-        <v>171</v>
-      </c>
-      <c r="K7" t="s">
-        <v>186</v>
-      </c>
-      <c r="L7" t="s">
-        <v>187</v>
-      </c>
-      <c r="M7" t="s">
-        <v>192</v>
       </c>
       <c r="N7">
         <v>5</v>
@@ -1425,10 +1371,10 @@
         <v>40</v>
       </c>
       <c r="P7" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="S7" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
@@ -1436,7 +1382,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
         <v>68</v>
@@ -1451,19 +1397,19 @@
         <v>70</v>
       </c>
       <c r="G8" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H8" t="s">
+        <v>152</v>
+      </c>
+      <c r="K8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L8" t="s">
+        <v>169</v>
+      </c>
+      <c r="M8" t="s">
         <v>171</v>
-      </c>
-      <c r="K8" t="s">
-        <v>189</v>
-      </c>
-      <c r="L8" t="s">
-        <v>188</v>
-      </c>
-      <c r="M8" t="s">
-        <v>190</v>
       </c>
       <c r="N8">
         <v>5</v>
@@ -1472,10 +1418,10 @@
         <v>25</v>
       </c>
       <c r="P8" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="S8" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
@@ -1483,7 +1429,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C9" t="s">
         <v>68</v>
@@ -1498,19 +1444,19 @@
         <v>69</v>
       </c>
       <c r="G9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H9" t="s">
+        <v>152</v>
+      </c>
+      <c r="K9" t="s">
+        <v>170</v>
+      </c>
+      <c r="L9" t="s">
+        <v>169</v>
+      </c>
+      <c r="M9" t="s">
         <v>173</v>
-      </c>
-      <c r="H9" t="s">
-        <v>171</v>
-      </c>
-      <c r="K9" t="s">
-        <v>189</v>
-      </c>
-      <c r="L9" t="s">
-        <v>188</v>
-      </c>
-      <c r="M9" t="s">
-        <v>192</v>
       </c>
       <c r="N9">
         <v>52</v>
@@ -1519,10 +1465,10 @@
         <v>57</v>
       </c>
       <c r="P9" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="S9" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T9" t="s">
         <v>68</v>
@@ -1536,7 +1482,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
         <v>68</v>
@@ -1551,19 +1497,19 @@
         <v>69</v>
       </c>
       <c r="G10" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H10" t="s">
+        <v>152</v>
+      </c>
+      <c r="K10" t="s">
+        <v>170</v>
+      </c>
+      <c r="L10" t="s">
+        <v>169</v>
+      </c>
+      <c r="M10" t="s">
         <v>171</v>
-      </c>
-      <c r="K10" t="s">
-        <v>189</v>
-      </c>
-      <c r="L10" t="s">
-        <v>188</v>
-      </c>
-      <c r="M10" t="s">
-        <v>190</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1572,10 +1518,10 @@
         <v>54</v>
       </c>
       <c r="P10" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="S10" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T10" t="s">
         <v>68</v>
@@ -1589,7 +1535,7 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="C11" t="s">
         <v>68</v>
@@ -1604,25 +1550,25 @@
         <v>69</v>
       </c>
       <c r="G11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H11" t="s">
+        <v>152</v>
+      </c>
+      <c r="K11" t="s">
+        <v>170</v>
+      </c>
+      <c r="L11" t="s">
+        <v>169</v>
+      </c>
+      <c r="M11" t="s">
         <v>173</v>
       </c>
-      <c r="H11" t="s">
-        <v>171</v>
-      </c>
-      <c r="K11" t="s">
-        <v>189</v>
-      </c>
-      <c r="L11" t="s">
-        <v>188</v>
-      </c>
-      <c r="M11" t="s">
-        <v>192</v>
-      </c>
       <c r="P11" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="S11" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
@@ -1630,7 +1576,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="C12" t="s">
         <v>68</v>
@@ -1645,19 +1591,19 @@
         <v>70</v>
       </c>
       <c r="G12" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H12" t="s">
+        <v>152</v>
+      </c>
+      <c r="K12" t="s">
+        <v>170</v>
+      </c>
+      <c r="L12" t="s">
+        <v>168</v>
+      </c>
+      <c r="M12" t="s">
         <v>171</v>
-      </c>
-      <c r="K12" t="s">
-        <v>189</v>
-      </c>
-      <c r="L12" t="s">
-        <v>187</v>
-      </c>
-      <c r="M12" t="s">
-        <v>190</v>
       </c>
       <c r="N12">
         <v>34</v>
@@ -1666,10 +1612,10 @@
         <v>56</v>
       </c>
       <c r="P12" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="S12" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T12" t="s">
         <v>68</v>
@@ -1683,13 +1629,13 @@
         <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="C13" t="s">
         <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>205</v>
       </c>
       <c r="E13" t="s">
         <v>68</v>
@@ -1698,19 +1644,19 @@
         <v>69</v>
       </c>
       <c r="G13" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K13" t="s">
+        <v>175</v>
+      </c>
+      <c r="L13" t="s">
+        <v>169</v>
+      </c>
+      <c r="M13" t="s">
         <v>171</v>
-      </c>
-      <c r="K13" t="s">
-        <v>194</v>
-      </c>
-      <c r="L13" t="s">
-        <v>188</v>
-      </c>
-      <c r="M13" t="s">
-        <v>190</v>
       </c>
       <c r="N13">
         <v>8</v>
@@ -1719,36 +1665,10 @@
         <v>29</v>
       </c>
       <c r="P13" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="S13" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" t="s">
-        <v>168</v>
-      </c>
-      <c r="F14" t="s">
-        <v>168</v>
-      </c>
-      <c r="G14" t="s">
-        <v>168</v>
-      </c>
-      <c r="H14" t="s">
-        <v>171</v>
-      </c>
-      <c r="L14" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
@@ -1756,13 +1676,13 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="C15" t="s">
         <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>205</v>
       </c>
       <c r="E15" t="s">
         <v>68</v>
@@ -1771,19 +1691,19 @@
         <v>70</v>
       </c>
       <c r="G15" t="s">
+        <v>154</v>
+      </c>
+      <c r="H15" t="s">
+        <v>152</v>
+      </c>
+      <c r="K15" t="s">
+        <v>170</v>
+      </c>
+      <c r="L15" t="s">
+        <v>169</v>
+      </c>
+      <c r="M15" t="s">
         <v>173</v>
-      </c>
-      <c r="H15" t="s">
-        <v>171</v>
-      </c>
-      <c r="K15" t="s">
-        <v>189</v>
-      </c>
-      <c r="L15" t="s">
-        <v>188</v>
-      </c>
-      <c r="M15" t="s">
-        <v>192</v>
       </c>
       <c r="N15">
         <v>17</v>
@@ -1792,10 +1712,10 @@
         <v>25</v>
       </c>
       <c r="P15" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="S15" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="T15" t="s">
         <v>68</v>
@@ -1809,7 +1729,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="C16" t="s">
         <v>68</v>
@@ -1824,19 +1744,19 @@
         <v>70</v>
       </c>
       <c r="G16" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H16" t="s">
+        <v>152</v>
+      </c>
+      <c r="K16" t="s">
+        <v>167</v>
+      </c>
+      <c r="L16" t="s">
+        <v>169</v>
+      </c>
+      <c r="M16" t="s">
         <v>171</v>
-      </c>
-      <c r="K16" t="s">
-        <v>186</v>
-      </c>
-      <c r="L16" t="s">
-        <v>188</v>
-      </c>
-      <c r="M16" t="s">
-        <v>190</v>
       </c>
       <c r="N16">
         <v>19</v>
@@ -1845,10 +1765,10 @@
         <v>24</v>
       </c>
       <c r="P16" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="S16" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T16" t="s">
         <v>68</v>
@@ -1859,7 +1779,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="C17" t="s">
         <v>68</v>
@@ -1874,19 +1794,19 @@
         <v>70</v>
       </c>
       <c r="G17" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H17" t="s">
+        <v>152</v>
+      </c>
+      <c r="K17" t="s">
+        <v>170</v>
+      </c>
+      <c r="L17" t="s">
+        <v>169</v>
+      </c>
+      <c r="M17" t="s">
         <v>171</v>
-      </c>
-      <c r="K17" t="s">
-        <v>189</v>
-      </c>
-      <c r="L17" t="s">
-        <v>188</v>
-      </c>
-      <c r="M17" t="s">
-        <v>190</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -1895,10 +1815,10 @@
         <v>35</v>
       </c>
       <c r="P17" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="S17" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="T17" t="s">
         <v>68</v>
@@ -1912,7 +1832,7 @@
         <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="C18" t="s">
         <v>68</v>
@@ -1921,10 +1841,10 @@
         <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H18" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
@@ -1932,7 +1852,7 @@
         <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="C19" t="s">
         <v>68</v>
@@ -1941,10 +1861,10 @@
         <v>69</v>
       </c>
       <c r="G19" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H19" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
@@ -1952,7 +1872,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
         <v>68</v>
@@ -1967,19 +1887,19 @@
         <v>70</v>
       </c>
       <c r="G20" t="s">
+        <v>154</v>
+      </c>
+      <c r="H20" t="s">
+        <v>152</v>
+      </c>
+      <c r="K20" t="s">
+        <v>170</v>
+      </c>
+      <c r="L20" t="s">
+        <v>168</v>
+      </c>
+      <c r="M20" t="s">
         <v>173</v>
-      </c>
-      <c r="H20" t="s">
-        <v>171</v>
-      </c>
-      <c r="K20" t="s">
-        <v>189</v>
-      </c>
-      <c r="L20" t="s">
-        <v>187</v>
-      </c>
-      <c r="M20" t="s">
-        <v>192</v>
       </c>
       <c r="N20">
         <v>20</v>
@@ -1988,42 +1908,16 @@
         <v>48</v>
       </c>
       <c r="P20" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="S20" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="T20" t="s">
         <v>68</v>
       </c>
       <c r="V20" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" t="s">
-        <v>148</v>
-      </c>
-      <c r="C21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" t="s">
-        <v>168</v>
-      </c>
-      <c r="F21" t="s">
-        <v>168</v>
-      </c>
-      <c r="G21" t="s">
-        <v>168</v>
-      </c>
-      <c r="H21" t="s">
-        <v>171</v>
-      </c>
-      <c r="L21" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
@@ -2031,7 +1925,7 @@
         <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C22" t="s">
         <v>68</v>
@@ -2040,10 +1934,10 @@
         <v>70</v>
       </c>
       <c r="G22" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H22" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
@@ -2051,7 +1945,7 @@
         <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="C23" t="s">
         <v>68</v>
@@ -2060,39 +1954,10 @@
         <v>69</v>
       </c>
       <c r="G23" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H23" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B24" t="s">
-        <v>145</v>
-      </c>
-      <c r="C24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" t="s">
-        <v>168</v>
-      </c>
-      <c r="F24" t="s">
-        <v>168</v>
-      </c>
-      <c r="G24" t="s">
-        <v>168</v>
-      </c>
-      <c r="H24" t="s">
-        <v>171</v>
-      </c>
-      <c r="L24" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
@@ -2100,7 +1965,7 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="C25" t="s">
         <v>68</v>
@@ -2115,19 +1980,19 @@
         <v>70</v>
       </c>
       <c r="G25" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H25" t="s">
+        <v>152</v>
+      </c>
+      <c r="K25" t="s">
+        <v>170</v>
+      </c>
+      <c r="L25" t="s">
+        <v>168</v>
+      </c>
+      <c r="M25" t="s">
         <v>171</v>
-      </c>
-      <c r="K25" t="s">
-        <v>189</v>
-      </c>
-      <c r="L25" t="s">
-        <v>187</v>
-      </c>
-      <c r="M25" t="s">
-        <v>190</v>
       </c>
       <c r="N25">
         <v>27</v>
@@ -2136,10 +2001,10 @@
         <v>39</v>
       </c>
       <c r="P25" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="S25" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="T25" t="s">
         <v>68</v>
@@ -2153,7 +2018,7 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="C26" t="s">
         <v>68</v>
@@ -2168,19 +2033,19 @@
         <v>70</v>
       </c>
       <c r="G26" t="s">
+        <v>154</v>
+      </c>
+      <c r="H26" t="s">
+        <v>152</v>
+      </c>
+      <c r="K26" t="s">
+        <v>170</v>
+      </c>
+      <c r="L26" t="s">
+        <v>169</v>
+      </c>
+      <c r="M26" t="s">
         <v>173</v>
-      </c>
-      <c r="H26" t="s">
-        <v>171</v>
-      </c>
-      <c r="K26" t="s">
-        <v>189</v>
-      </c>
-      <c r="L26" t="s">
-        <v>188</v>
-      </c>
-      <c r="M26" t="s">
-        <v>192</v>
       </c>
       <c r="N26">
         <v>24</v>
@@ -2189,10 +2054,10 @@
         <v>45</v>
       </c>
       <c r="P26" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="S26" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="T26" t="s">
         <v>68</v>
@@ -2206,7 +2071,7 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="C27" t="s">
         <v>68</v>
@@ -2221,19 +2086,19 @@
         <v>70</v>
       </c>
       <c r="G27" t="s">
+        <v>154</v>
+      </c>
+      <c r="H27" t="s">
+        <v>152</v>
+      </c>
+      <c r="K27" t="s">
+        <v>170</v>
+      </c>
+      <c r="L27" t="s">
+        <v>168</v>
+      </c>
+      <c r="M27" t="s">
         <v>173</v>
-      </c>
-      <c r="H27" t="s">
-        <v>171</v>
-      </c>
-      <c r="K27" t="s">
-        <v>189</v>
-      </c>
-      <c r="L27" t="s">
-        <v>187</v>
-      </c>
-      <c r="M27" t="s">
-        <v>192</v>
       </c>
       <c r="N27">
         <v>5</v>
@@ -2242,10 +2107,10 @@
         <v>36</v>
       </c>
       <c r="P27" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="S27" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="T27" t="s">
         <v>68</v>
@@ -2256,7 +2121,7 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="C28" t="s">
         <v>68</v>
@@ -2271,19 +2136,19 @@
         <v>70</v>
       </c>
       <c r="G28" t="s">
+        <v>154</v>
+      </c>
+      <c r="H28" t="s">
+        <v>152</v>
+      </c>
+      <c r="K28" t="s">
+        <v>170</v>
+      </c>
+      <c r="L28" t="s">
+        <v>168</v>
+      </c>
+      <c r="M28" t="s">
         <v>173</v>
-      </c>
-      <c r="H28" t="s">
-        <v>171</v>
-      </c>
-      <c r="K28" t="s">
-        <v>189</v>
-      </c>
-      <c r="L28" t="s">
-        <v>187</v>
-      </c>
-      <c r="M28" t="s">
-        <v>192</v>
       </c>
       <c r="N28">
         <v>28</v>
@@ -2292,10 +2157,10 @@
         <v>40</v>
       </c>
       <c r="P28" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="S28" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T28" t="s">
         <v>68</v>
@@ -2309,7 +2174,7 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
         <v>68</v>
@@ -2324,19 +2189,19 @@
         <v>69</v>
       </c>
       <c r="G29" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H29" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="K29" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="L29" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="M29" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N29">
         <v>0</v>
@@ -2345,10 +2210,10 @@
         <v>21</v>
       </c>
       <c r="P29" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="Q29" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="T29" t="s">
         <v>68</v>
@@ -2362,7 +2227,7 @@
         <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="C30" t="s">
         <v>68</v>
@@ -2371,10 +2236,10 @@
         <v>71</v>
       </c>
       <c r="G30" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H30" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -2382,9 +2247,12 @@
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="C31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" t="s">
         <v>68</v>
       </c>
       <c r="E31" t="s">
@@ -2394,10 +2262,22 @@
         <v>69</v>
       </c>
       <c r="G31" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H31" t="s">
-        <v>171</v>
+        <v>152</v>
+      </c>
+      <c r="N31">
+        <v>23</v>
+      </c>
+      <c r="O31">
+        <v>42</v>
+      </c>
+      <c r="P31" t="s">
+        <v>174</v>
+      </c>
+      <c r="S31" t="s">
+        <v>202</v>
       </c>
       <c r="T31" t="s">
         <v>68</v>
@@ -2411,7 +2291,7 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="C32" t="s">
         <v>68</v>
@@ -2426,25 +2306,25 @@
         <v>70</v>
       </c>
       <c r="G32" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H32" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I32" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="J32" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="K32" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="L32" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="M32" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N32">
         <v>42</v>
@@ -2453,13 +2333,13 @@
         <v>59</v>
       </c>
       <c r="P32" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="Q32" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S32" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T32" t="s">
         <v>68</v>
@@ -2473,7 +2353,7 @@
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="C33" t="s">
         <v>68</v>
@@ -2488,25 +2368,25 @@
         <v>70</v>
       </c>
       <c r="G33" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H33" t="s">
+        <v>151</v>
+      </c>
+      <c r="I33" t="s">
+        <v>188</v>
+      </c>
+      <c r="J33" t="s">
+        <v>187</v>
+      </c>
+      <c r="K33" t="s">
         <v>170</v>
       </c>
-      <c r="I33" t="s">
-        <v>208</v>
-      </c>
-      <c r="J33" t="s">
-        <v>207</v>
-      </c>
-      <c r="K33" t="s">
-        <v>189</v>
-      </c>
       <c r="L33" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M33" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N33">
         <v>12</v>
@@ -2515,42 +2395,19 @@
         <v>39</v>
       </c>
       <c r="P33" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="Q33" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="S33" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T33" t="s">
         <v>68</v>
       </c>
       <c r="V33" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" t="s">
-        <v>136</v>
-      </c>
-      <c r="C34" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" t="s">
-        <v>168</v>
-      </c>
-      <c r="F34" t="s">
-        <v>168</v>
-      </c>
-      <c r="G34" t="s">
-        <v>168</v>
-      </c>
-      <c r="L34" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.2">
@@ -2558,19 +2415,34 @@
         <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" t="s">
         <v>68</v>
       </c>
       <c r="F35" t="s">
         <v>70</v>
       </c>
       <c r="G35" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H35" t="s">
-        <v>171</v>
+        <v>152</v>
+      </c>
+      <c r="N35">
+        <v>33</v>
+      </c>
+      <c r="O35">
+        <v>36</v>
+      </c>
+      <c r="P35" t="s">
+        <v>172</v>
       </c>
       <c r="T35" t="s">
         <v>68</v>
@@ -2581,7 +2453,7 @@
         <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C36" t="s">
         <v>68</v>
@@ -2596,10 +2468,19 @@
         <v>70</v>
       </c>
       <c r="G36" t="s">
+        <v>153</v>
+      </c>
+      <c r="H36" t="s">
+        <v>152</v>
+      </c>
+      <c r="N36">
+        <v>44</v>
+      </c>
+      <c r="O36">
+        <v>45</v>
+      </c>
+      <c r="P36" t="s">
         <v>172</v>
-      </c>
-      <c r="H36" t="s">
-        <v>171</v>
       </c>
       <c r="T36" t="s">
         <v>68</v>
@@ -2613,7 +2494,7 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="C37" t="s">
         <v>68</v>
@@ -2628,19 +2509,19 @@
         <v>71</v>
       </c>
       <c r="G37" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H37" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="K37" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="L37" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M37" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="N37">
         <v>48</v>
@@ -2649,7 +2530,7 @@
         <v>57</v>
       </c>
       <c r="P37" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="T37" t="s">
         <v>68</v>
@@ -2663,7 +2544,7 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C38" t="s">
         <v>68</v>
@@ -2678,42 +2559,22 @@
         <v>71</v>
       </c>
       <c r="G38" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H38" t="s">
-        <v>171</v>
+        <v>152</v>
+      </c>
+      <c r="N38">
+        <v>22</v>
+      </c>
+      <c r="O38">
+        <v>26</v>
+      </c>
+      <c r="P38" t="s">
+        <v>174</v>
       </c>
       <c r="T38" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>86</v>
-      </c>
-      <c r="B39" t="s">
-        <v>131</v>
-      </c>
-      <c r="C39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E39" t="s">
-        <v>168</v>
-      </c>
-      <c r="F39" t="s">
-        <v>168</v>
-      </c>
-      <c r="G39" t="s">
-        <v>168</v>
-      </c>
-      <c r="H39" t="s">
-        <v>170</v>
-      </c>
-      <c r="L39" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
@@ -2721,7 +2582,7 @@
         <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C40" t="s">
         <v>68</v>
@@ -2736,25 +2597,25 @@
         <v>70</v>
       </c>
       <c r="G40" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H40" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I40" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="J40" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="K40" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="L40" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M40" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="N40">
         <v>20</v>
@@ -2763,13 +2624,13 @@
         <v>46</v>
       </c>
       <c r="P40" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="Q40" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S40" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T40" t="s">
         <v>68</v>
@@ -2783,19 +2644,22 @@
         <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C41" t="s">
         <v>68</v>
+      </c>
+      <c r="E41" t="s">
+        <v>204</v>
       </c>
       <c r="F41" t="s">
         <v>69</v>
       </c>
       <c r="G41" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H41" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="T41" t="s">
         <v>68</v>
@@ -2809,7 +2673,7 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C42" t="s">
         <v>68</v>
@@ -2824,19 +2688,19 @@
         <v>69</v>
       </c>
       <c r="G42" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H42" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="K42" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="L42" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M42" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="N42">
         <v>47</v>
@@ -2845,13 +2709,13 @@
         <v>52</v>
       </c>
       <c r="P42" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="Q42" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S42" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T42" t="s">
         <v>68</v>
@@ -2865,7 +2729,7 @@
         <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="C43" t="s">
         <v>68</v>
@@ -2880,10 +2744,25 @@
         <v>71</v>
       </c>
       <c r="G43" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H43" t="s">
-        <v>170</v>
+        <v>151</v>
+      </c>
+      <c r="K43" t="s">
+        <v>167</v>
+      </c>
+      <c r="M43" t="s">
+        <v>171</v>
+      </c>
+      <c r="N43">
+        <v>8</v>
+      </c>
+      <c r="O43">
+        <v>32</v>
+      </c>
+      <c r="P43" t="s">
+        <v>172</v>
       </c>
       <c r="T43" t="s">
         <v>68</v>
@@ -2897,10 +2776,13 @@
         <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C44" t="s">
         <v>68</v>
+      </c>
+      <c r="D44" t="s">
+        <v>205</v>
       </c>
       <c r="E44" t="s">
         <v>68</v>
@@ -2909,25 +2791,25 @@
         <v>69</v>
       </c>
       <c r="G44" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H44" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I44" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="J44" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="K44" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="L44" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="M44" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="N44">
         <v>34</v>
@@ -2936,48 +2818,19 @@
         <v>37</v>
       </c>
       <c r="P44" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="Q44" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S44" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T44" t="s">
         <v>68</v>
       </c>
       <c r="V44" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>87</v>
-      </c>
-      <c r="B45" t="s">
-        <v>128</v>
-      </c>
-      <c r="C45" t="s">
-        <v>68</v>
-      </c>
-      <c r="D45" t="s">
-        <v>68</v>
-      </c>
-      <c r="E45" t="s">
-        <v>168</v>
-      </c>
-      <c r="F45" t="s">
-        <v>168</v>
-      </c>
-      <c r="G45" t="s">
-        <v>168</v>
-      </c>
-      <c r="H45" t="s">
-        <v>170</v>
-      </c>
-      <c r="L45" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.2">
@@ -2985,7 +2838,7 @@
         <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C46" t="s">
         <v>68</v>
@@ -3000,25 +2853,25 @@
         <v>69</v>
       </c>
       <c r="G46" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H46" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I46" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="J46" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="K46" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="L46" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M46" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N46">
         <v>29</v>
@@ -3027,13 +2880,13 @@
         <v>38</v>
       </c>
       <c r="P46" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="Q46" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S46" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="T46" t="s">
         <v>68</v>
@@ -3047,7 +2900,7 @@
         <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C47" t="s">
         <v>68</v>
@@ -3062,25 +2915,25 @@
         <v>70</v>
       </c>
       <c r="G47" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H47" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I47" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="J47" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="K47" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="L47" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M47" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N47">
         <v>0</v>
@@ -3089,13 +2942,13 @@
         <v>20</v>
       </c>
       <c r="P47" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="Q47" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="S47" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="T47" t="s">
         <v>68</v>
@@ -3109,7 +2962,7 @@
         <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C48" t="s">
         <v>68</v>
@@ -3124,25 +2977,25 @@
         <v>70</v>
       </c>
       <c r="G48" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H48" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I48" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="J48" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="K48" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="L48" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M48" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="N48">
         <v>26</v>
@@ -3151,13 +3004,13 @@
         <v>47</v>
       </c>
       <c r="P48" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="Q48" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S48" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T48" t="s">
         <v>68</v>
@@ -3171,7 +3024,7 @@
         <v>41</v>
       </c>
       <c r="B49" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C49" t="s">
         <v>68</v>
@@ -3186,25 +3039,25 @@
         <v>69</v>
       </c>
       <c r="G49" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H49" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I49" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="J49" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="K49" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="L49" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="M49" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="N49">
         <v>14</v>
@@ -3213,13 +3066,13 @@
         <v>30</v>
       </c>
       <c r="P49" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="Q49" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S49" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T49" t="s">
         <v>68</v>
@@ -3233,54 +3086,43 @@
         <v>42</v>
       </c>
       <c r="B50" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C50" t="s">
+        <v>68</v>
+      </c>
+      <c r="E50" t="s">
         <v>68</v>
       </c>
       <c r="F50" t="s">
         <v>69</v>
       </c>
       <c r="G50" t="s">
+        <v>153</v>
+      </c>
+      <c r="H50" t="s">
+        <v>151</v>
+      </c>
+      <c r="M50" t="s">
+        <v>171</v>
+      </c>
+      <c r="N50">
+        <v>15</v>
+      </c>
+      <c r="O50">
+        <v>30</v>
+      </c>
+      <c r="P50" t="s">
         <v>172</v>
       </c>
-      <c r="H50" t="s">
-        <v>170</v>
+      <c r="Q50" t="s">
+        <v>203</v>
       </c>
       <c r="T50" t="s">
         <v>68</v>
       </c>
       <c r="V50" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" t="s">
-        <v>125</v>
-      </c>
-      <c r="C51" t="s">
-        <v>68</v>
-      </c>
-      <c r="D51" t="s">
-        <v>68</v>
-      </c>
-      <c r="E51" t="s">
-        <v>168</v>
-      </c>
-      <c r="F51" t="s">
-        <v>168</v>
-      </c>
-      <c r="G51" t="s">
-        <v>168</v>
-      </c>
-      <c r="H51" t="s">
-        <v>170</v>
-      </c>
-      <c r="L51" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
@@ -3288,19 +3130,40 @@
         <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" t="s">
+        <v>68</v>
+      </c>
+      <c r="E52" t="s">
         <v>68</v>
       </c>
       <c r="F52" t="s">
         <v>71</v>
       </c>
       <c r="G52" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H52" t="s">
-        <v>170</v>
+        <v>151</v>
+      </c>
+      <c r="M52" t="s">
+        <v>171</v>
+      </c>
+      <c r="N52">
+        <v>5</v>
+      </c>
+      <c r="O52">
+        <v>31</v>
+      </c>
+      <c r="P52" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>202</v>
       </c>
       <c r="T52" t="s">
         <v>68</v>
@@ -3314,19 +3177,40 @@
         <v>45</v>
       </c>
       <c r="B53" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" t="s">
         <v>68</v>
       </c>
       <c r="F53" t="s">
         <v>70</v>
       </c>
       <c r="G53" t="s">
+        <v>154</v>
+      </c>
+      <c r="H53" t="s">
+        <v>151</v>
+      </c>
+      <c r="K53" t="s">
+        <v>170</v>
+      </c>
+      <c r="M53" t="s">
         <v>173</v>
       </c>
-      <c r="H53" t="s">
-        <v>170</v>
+      <c r="N53">
+        <v>4</v>
+      </c>
+      <c r="O53">
+        <v>16</v>
+      </c>
+      <c r="P53" t="s">
+        <v>172</v>
       </c>
       <c r="T53" t="s">
         <v>68</v>
@@ -3340,10 +3224,13 @@
         <v>44</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C54" t="s">
         <v>68</v>
+      </c>
+      <c r="D54" t="s">
+        <v>205</v>
       </c>
       <c r="E54" t="s">
         <v>68</v>
@@ -3352,13 +3239,25 @@
         <v>70</v>
       </c>
       <c r="G54" t="s">
+        <v>153</v>
+      </c>
+      <c r="H54" t="s">
+        <v>151</v>
+      </c>
+      <c r="M54" t="s">
+        <v>171</v>
+      </c>
+      <c r="N54">
+        <v>16</v>
+      </c>
+      <c r="O54">
+        <v>23</v>
+      </c>
+      <c r="P54" t="s">
         <v>172</v>
       </c>
-      <c r="H54" t="s">
-        <v>170</v>
-      </c>
       <c r="Q54" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T54" t="s">
         <v>68</v>
@@ -3372,7 +3271,7 @@
         <v>46</v>
       </c>
       <c r="B55" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C55" t="s">
         <v>68</v>
@@ -3387,25 +3286,25 @@
         <v>70</v>
       </c>
       <c r="G55" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H55" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I55" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="J55" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="K55" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="L55" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="M55" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N55">
         <v>4</v>
@@ -3414,13 +3313,13 @@
         <v>17</v>
       </c>
       <c r="P55" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="Q55" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S55" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T55" t="s">
         <v>68</v>
@@ -3434,7 +3333,7 @@
         <v>47</v>
       </c>
       <c r="B56" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C56" t="s">
         <v>68</v>
@@ -3449,60 +3348,37 @@
         <v>70</v>
       </c>
       <c r="G56" t="s">
+        <v>153</v>
+      </c>
+      <c r="H56" t="s">
+        <v>151</v>
+      </c>
+      <c r="I56" t="s">
+        <v>194</v>
+      </c>
+      <c r="K56" t="s">
+        <v>182</v>
+      </c>
+      <c r="L56" t="s">
+        <v>168</v>
+      </c>
+      <c r="M56" t="s">
+        <v>173</v>
+      </c>
+      <c r="P56" t="s">
         <v>172</v>
       </c>
-      <c r="H56" t="s">
-        <v>170</v>
-      </c>
-      <c r="I56" t="s">
-        <v>214</v>
-      </c>
-      <c r="K56" t="s">
+      <c r="Q56" t="s">
+        <v>203</v>
+      </c>
+      <c r="S56" t="s">
         <v>202</v>
       </c>
-      <c r="L56" t="s">
-        <v>187</v>
-      </c>
-      <c r="M56" t="s">
-        <v>192</v>
-      </c>
-      <c r="P56" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>223</v>
-      </c>
-      <c r="S56" t="s">
-        <v>222</v>
-      </c>
       <c r="T56" t="s">
         <v>68</v>
       </c>
       <c r="V56" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>89</v>
-      </c>
-      <c r="B57" t="s">
-        <v>122</v>
-      </c>
-      <c r="E57" t="s">
-        <v>168</v>
-      </c>
-      <c r="F57" t="s">
-        <v>168</v>
-      </c>
-      <c r="G57" t="s">
-        <v>168</v>
-      </c>
-      <c r="H57" t="s">
-        <v>170</v>
-      </c>
-      <c r="L57" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
@@ -3510,7 +3386,7 @@
         <v>48</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C58" t="s">
         <v>68</v>
@@ -3525,25 +3401,25 @@
         <v>70</v>
       </c>
       <c r="G58" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H58" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I58" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="J58" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="K58" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="L58" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M58" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="N58">
         <v>16</v>
@@ -3552,13 +3428,13 @@
         <v>25</v>
       </c>
       <c r="P58" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="Q58" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S58" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T58" t="s">
         <v>68</v>
@@ -3572,7 +3448,7 @@
         <v>49</v>
       </c>
       <c r="B59" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C59" t="s">
         <v>68</v>
@@ -3587,25 +3463,25 @@
         <v>69</v>
       </c>
       <c r="G59" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H59" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I59" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="J59" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="K59" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="L59" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="M59" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="N59">
         <v>7</v>
@@ -3614,13 +3490,13 @@
         <v>32</v>
       </c>
       <c r="P59" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="Q59" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S59" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="T59" t="s">
         <v>68</v>
@@ -3634,19 +3510,43 @@
         <v>50</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C60" t="s">
+        <v>68</v>
+      </c>
+      <c r="D60" t="s">
+        <v>68</v>
+      </c>
+      <c r="E60" t="s">
         <v>68</v>
       </c>
       <c r="F60" t="s">
         <v>71</v>
       </c>
       <c r="G60" t="s">
+        <v>154</v>
+      </c>
+      <c r="H60" t="s">
+        <v>151</v>
+      </c>
+      <c r="K60" t="s">
+        <v>170</v>
+      </c>
+      <c r="M60" t="s">
         <v>173</v>
       </c>
-      <c r="H60" t="s">
-        <v>170</v>
+      <c r="N60">
+        <v>15</v>
+      </c>
+      <c r="O60">
+        <v>45</v>
+      </c>
+      <c r="P60" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>203</v>
       </c>
       <c r="T60" t="s">
         <v>68</v>
@@ -3660,22 +3560,43 @@
         <v>51</v>
       </c>
       <c r="B61" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C61" t="s">
         <v>68</v>
       </c>
       <c r="D61" t="s">
+        <v>68</v>
+      </c>
+      <c r="E61" t="s">
         <v>68</v>
       </c>
       <c r="F61" t="s">
         <v>69</v>
       </c>
       <c r="G61" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H61" t="s">
-        <v>170</v>
+        <v>151</v>
+      </c>
+      <c r="K61" t="s">
+        <v>181</v>
+      </c>
+      <c r="M61" t="s">
+        <v>173</v>
+      </c>
+      <c r="N61">
+        <v>21</v>
+      </c>
+      <c r="O61">
+        <v>35</v>
+      </c>
+      <c r="P61" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>203</v>
       </c>
       <c r="T61" t="s">
         <v>68</v>
@@ -3689,7 +3610,7 @@
         <v>52</v>
       </c>
       <c r="B62" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C62" t="s">
         <v>68</v>
@@ -3704,25 +3625,25 @@
         <v>70</v>
       </c>
       <c r="G62" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H62" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I62" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="J62" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="K62" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="L62" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M62" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="N62">
         <v>32</v>
@@ -3731,13 +3652,13 @@
         <v>42</v>
       </c>
       <c r="P62" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="Q62" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S62" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="T62" t="s">
         <v>68</v>
@@ -3751,7 +3672,7 @@
         <v>53</v>
       </c>
       <c r="B63" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C63" t="s">
         <v>68</v>
@@ -3766,25 +3687,25 @@
         <v>70</v>
       </c>
       <c r="G63" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H63" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I63" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="J63" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="K63" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="L63" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M63" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N63">
         <v>14</v>
@@ -3793,13 +3714,13 @@
         <v>34</v>
       </c>
       <c r="P63" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="Q63" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S63" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="T63" t="s">
         <v>68</v>
@@ -3813,7 +3734,7 @@
         <v>54</v>
       </c>
       <c r="B64" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C64" t="s">
         <v>68</v>
@@ -3828,25 +3749,25 @@
         <v>70</v>
       </c>
       <c r="G64" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H64" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I64" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="J64" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="K64" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="L64" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="M64" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="N64">
         <v>12</v>
@@ -3855,7 +3776,7 @@
         <v>21</v>
       </c>
       <c r="P64" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="T64" t="s">
         <v>68</v>
@@ -3869,22 +3790,40 @@
         <v>55</v>
       </c>
       <c r="B65" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C65" t="s">
         <v>68</v>
       </c>
       <c r="D65" t="s">
+        <v>68</v>
+      </c>
+      <c r="E65" t="s">
         <v>68</v>
       </c>
       <c r="F65" t="s">
         <v>70</v>
       </c>
       <c r="G65" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H65" t="s">
+        <v>151</v>
+      </c>
+      <c r="K65" t="s">
         <v>170</v>
+      </c>
+      <c r="N65">
+        <v>4</v>
+      </c>
+      <c r="O65">
+        <v>26</v>
+      </c>
+      <c r="P65" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>202</v>
       </c>
       <c r="T65" t="s">
         <v>68</v>
@@ -3898,7 +3837,7 @@
         <v>56</v>
       </c>
       <c r="B66" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C66" t="s">
         <v>68</v>
@@ -3913,25 +3852,25 @@
         <v>69</v>
       </c>
       <c r="G66" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H66" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I66" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="J66" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="K66" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="L66" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="M66" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="N66">
         <v>3</v>
@@ -3940,13 +3879,13 @@
         <v>21</v>
       </c>
       <c r="P66" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="Q66" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S66" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.2">
@@ -3954,7 +3893,7 @@
         <v>57</v>
       </c>
       <c r="B67" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C67" t="s">
         <v>68</v>
@@ -3969,25 +3908,25 @@
         <v>69</v>
       </c>
       <c r="G67" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H67" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I67" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="J67" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="K67" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="L67" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M67" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="N67">
         <v>6</v>
@@ -3996,13 +3935,13 @@
         <v>50</v>
       </c>
       <c r="P67" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="Q67" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S67" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.2">
@@ -4010,7 +3949,7 @@
         <v>58</v>
       </c>
       <c r="B68" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C68" t="s">
         <v>68</v>
@@ -4025,25 +3964,25 @@
         <v>69</v>
       </c>
       <c r="G68" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H68" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I68" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="J68" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="K68" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="L68" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M68" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="N68">
         <v>2</v>
@@ -4052,13 +3991,13 @@
         <v>28</v>
       </c>
       <c r="P68" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="Q68" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S68" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.2">
@@ -4066,7 +4005,7 @@
         <v>59</v>
       </c>
       <c r="B69" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C69" t="s">
         <v>68</v>
@@ -4081,25 +4020,25 @@
         <v>70</v>
       </c>
       <c r="G69" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H69" t="s">
+        <v>151</v>
+      </c>
+      <c r="I69" t="s">
+        <v>185</v>
+      </c>
+      <c r="J69" t="s">
+        <v>190</v>
+      </c>
+      <c r="K69" t="s">
         <v>170</v>
       </c>
-      <c r="I69" t="s">
-        <v>205</v>
-      </c>
-      <c r="J69" t="s">
-        <v>210</v>
-      </c>
-      <c r="K69" t="s">
-        <v>189</v>
-      </c>
       <c r="L69" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="M69" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N69">
         <v>12</v>
@@ -4108,10 +4047,10 @@
         <v>24</v>
       </c>
       <c r="P69" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="Q69" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.2">
@@ -4119,7 +4058,7 @@
         <v>60</v>
       </c>
       <c r="B70" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C70" t="s">
         <v>68</v>
@@ -4134,25 +4073,25 @@
         <v>70</v>
       </c>
       <c r="G70" t="s">
+        <v>154</v>
+      </c>
+      <c r="H70" t="s">
+        <v>151</v>
+      </c>
+      <c r="I70" t="s">
+        <v>197</v>
+      </c>
+      <c r="J70" t="s">
+        <v>196</v>
+      </c>
+      <c r="K70" t="s">
+        <v>170</v>
+      </c>
+      <c r="L70" t="s">
+        <v>168</v>
+      </c>
+      <c r="M70" t="s">
         <v>173</v>
-      </c>
-      <c r="H70" t="s">
-        <v>170</v>
-      </c>
-      <c r="I70" t="s">
-        <v>217</v>
-      </c>
-      <c r="J70" t="s">
-        <v>216</v>
-      </c>
-      <c r="K70" t="s">
-        <v>189</v>
-      </c>
-      <c r="L70" t="s">
-        <v>187</v>
-      </c>
-      <c r="M70" t="s">
-        <v>192</v>
       </c>
       <c r="N70">
         <v>5</v>
@@ -4161,13 +4100,13 @@
         <v>42</v>
       </c>
       <c r="P70" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="Q70" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S70" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.2">
@@ -4175,7 +4114,7 @@
         <v>61</v>
       </c>
       <c r="B71" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C71" t="s">
         <v>68</v>
@@ -4190,19 +4129,19 @@
         <v>71</v>
       </c>
       <c r="G71" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H71" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="K71" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="L71" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M71" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N71">
         <v>13</v>
@@ -4211,10 +4150,10 @@
         <v>20</v>
       </c>
       <c r="P71" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="Q71" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.2">
@@ -4222,7 +4161,7 @@
         <v>62</v>
       </c>
       <c r="B72" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C72" t="s">
         <v>68</v>
@@ -4237,19 +4176,19 @@
         <v>70</v>
       </c>
       <c r="G72" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H72" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="K72" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="L72" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M72" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N72">
         <v>2</v>
@@ -4258,10 +4197,10 @@
         <v>28</v>
       </c>
       <c r="P72" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="Q72" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.2">
@@ -4269,7 +4208,7 @@
         <v>63</v>
       </c>
       <c r="B73" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C73" t="s">
         <v>68</v>
@@ -4284,25 +4223,25 @@
         <v>71</v>
       </c>
       <c r="G73" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H73" t="s">
+        <v>151</v>
+      </c>
+      <c r="I73" t="s">
+        <v>190</v>
+      </c>
+      <c r="J73" t="s">
+        <v>195</v>
+      </c>
+      <c r="K73" t="s">
         <v>170</v>
       </c>
-      <c r="I73" t="s">
-        <v>210</v>
-      </c>
-      <c r="J73" t="s">
-        <v>215</v>
-      </c>
-      <c r="K73" t="s">
-        <v>189</v>
-      </c>
       <c r="L73" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M73" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N73">
         <v>16</v>
@@ -4311,42 +4250,13 @@
         <v>31</v>
       </c>
       <c r="P73" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="Q73" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S73" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>90</v>
-      </c>
-      <c r="B74" t="s">
-        <v>117</v>
-      </c>
-      <c r="C74" t="s">
-        <v>68</v>
-      </c>
-      <c r="D74" t="s">
-        <v>68</v>
-      </c>
-      <c r="E74" t="s">
-        <v>168</v>
-      </c>
-      <c r="F74" t="s">
-        <v>168</v>
-      </c>
-      <c r="G74" t="s">
-        <v>168</v>
-      </c>
-      <c r="H74" t="s">
-        <v>170</v>
-      </c>
-      <c r="L74" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.2">
@@ -4354,7 +4264,7 @@
         <v>64</v>
       </c>
       <c r="B75" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C75" t="s">
         <v>68</v>
@@ -4369,25 +4279,25 @@
         <v>70</v>
       </c>
       <c r="G75" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H75" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I75" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="J75" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="K75" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="L75" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M75" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N75">
         <v>9</v>
@@ -4396,13 +4306,13 @@
         <v>38</v>
       </c>
       <c r="P75" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="Q75" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S75" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.2">
@@ -4410,7 +4320,7 @@
         <v>65</v>
       </c>
       <c r="B76" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C76" t="s">
         <v>68</v>
@@ -4425,10 +4335,28 @@
         <v>71</v>
       </c>
       <c r="G76" t="s">
+        <v>153</v>
+      </c>
+      <c r="H76" t="s">
+        <v>151</v>
+      </c>
+      <c r="K76" t="s">
+        <v>181</v>
+      </c>
+      <c r="M76" t="s">
+        <v>173</v>
+      </c>
+      <c r="N76">
+        <v>18</v>
+      </c>
+      <c r="O76">
+        <v>25</v>
+      </c>
+      <c r="P76" t="s">
         <v>172</v>
       </c>
-      <c r="H76" t="s">
-        <v>170</v>
+      <c r="Q76" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.2">
@@ -4436,7 +4364,7 @@
         <v>66</v>
       </c>
       <c r="B77" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C77" t="s">
         <v>68</v>
@@ -4451,25 +4379,25 @@
         <v>69</v>
       </c>
       <c r="G77" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H77" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I77" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="J77" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="K77" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="L77" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="M77" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N77">
         <v>9</v>
@@ -4478,10 +4406,10 @@
         <v>24</v>
       </c>
       <c r="P77" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="Q77" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.2">
@@ -4489,34 +4417,40 @@
         <v>67</v>
       </c>
       <c r="B78" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C78" t="s">
         <v>68</v>
       </c>
+      <c r="D78" t="s">
+        <v>205</v>
+      </c>
       <c r="E78" t="s">
         <v>68</v>
       </c>
+      <c r="F78" t="s">
+        <v>70</v>
+      </c>
       <c r="G78" t="s">
+        <v>154</v>
+      </c>
+      <c r="H78" t="s">
+        <v>151</v>
+      </c>
+      <c r="I78" t="s">
+        <v>191</v>
+      </c>
+      <c r="J78" t="s">
+        <v>188</v>
+      </c>
+      <c r="K78" t="s">
+        <v>181</v>
+      </c>
+      <c r="L78" t="s">
+        <v>169</v>
+      </c>
+      <c r="M78" t="s">
         <v>173</v>
-      </c>
-      <c r="H78" t="s">
-        <v>170</v>
-      </c>
-      <c r="I78" t="s">
-        <v>211</v>
-      </c>
-      <c r="J78" t="s">
-        <v>208</v>
-      </c>
-      <c r="K78" t="s">
-        <v>201</v>
-      </c>
-      <c r="L78" t="s">
-        <v>188</v>
-      </c>
-      <c r="M78" t="s">
-        <v>192</v>
       </c>
       <c r="N78">
         <v>12</v>
@@ -4525,21 +4459,21 @@
         <v>25</v>
       </c>
       <c r="P78" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="Q78" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="S78" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="B79" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C79" t="s">
         <v>68</v>
@@ -4554,16 +4488,16 @@
         <v>71</v>
       </c>
       <c r="G79" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H79" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="K79" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="L79" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="N79">
         <v>23</v>
@@ -4572,18 +4506,18 @@
         <v>37</v>
       </c>
       <c r="P79" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="S79" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="B80" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C80" t="s">
         <v>68</v>
@@ -4598,16 +4532,16 @@
         <v>69</v>
       </c>
       <c r="G80" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H80" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="K80" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="L80" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="N80">
         <v>5</v>
@@ -4616,18 +4550,18 @@
         <v>36</v>
       </c>
       <c r="P80" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="S80" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="B81" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C81" t="s">
         <v>68</v>
@@ -4642,30 +4576,30 @@
         <v>69</v>
       </c>
       <c r="G81" t="s">
+        <v>154</v>
+      </c>
+      <c r="H81" t="s">
+        <v>152</v>
+      </c>
+      <c r="K81" t="s">
+        <v>170</v>
+      </c>
+      <c r="L81" t="s">
+        <v>168</v>
+      </c>
+      <c r="M81" t="s">
         <v>173</v>
       </c>
-      <c r="H81" t="s">
-        <v>171</v>
-      </c>
-      <c r="K81" t="s">
-        <v>189</v>
-      </c>
-      <c r="L81" t="s">
-        <v>187</v>
-      </c>
-      <c r="M81" t="s">
-        <v>192</v>
-      </c>
       <c r="P81" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="B82" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C82" t="s">
         <v>68</v>
@@ -4680,19 +4614,19 @@
         <v>69</v>
       </c>
       <c r="G82" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H82" t="s">
+        <v>152</v>
+      </c>
+      <c r="K82" t="s">
+        <v>170</v>
+      </c>
+      <c r="L82" t="s">
+        <v>169</v>
+      </c>
+      <c r="M82" t="s">
         <v>171</v>
-      </c>
-      <c r="K82" t="s">
-        <v>189</v>
-      </c>
-      <c r="L82" t="s">
-        <v>188</v>
-      </c>
-      <c r="M82" t="s">
-        <v>190</v>
       </c>
       <c r="N82">
         <v>31</v>
@@ -4701,18 +4635,18 @@
         <v>33</v>
       </c>
       <c r="P82" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="S82" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="B83" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C83" t="s">
         <v>68</v>
@@ -4727,16 +4661,16 @@
         <v>69</v>
       </c>
       <c r="G83" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H83" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="K83" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="L83" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="N83">
         <v>5</v>
@@ -4745,15 +4679,15 @@
         <v>10</v>
       </c>
       <c r="P83" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="B84" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C84" t="s">
         <v>68</v>
@@ -4768,30 +4702,30 @@
         <v>69</v>
       </c>
       <c r="G84" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="H84" t="s">
+        <v>152</v>
+      </c>
+      <c r="K84" t="s">
+        <v>170</v>
+      </c>
+      <c r="L84" t="s">
+        <v>169</v>
+      </c>
+      <c r="M84" t="s">
         <v>171</v>
       </c>
-      <c r="K84" t="s">
-        <v>189</v>
-      </c>
-      <c r="L84" t="s">
-        <v>188</v>
-      </c>
-      <c r="M84" t="s">
-        <v>190</v>
-      </c>
       <c r="P84" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="B85" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C85" t="s">
         <v>68</v>
@@ -4806,19 +4740,19 @@
         <v>69</v>
       </c>
       <c r="G85" t="s">
+        <v>154</v>
+      </c>
+      <c r="H85" t="s">
+        <v>152</v>
+      </c>
+      <c r="K85" t="s">
+        <v>180</v>
+      </c>
+      <c r="L85" t="s">
+        <v>169</v>
+      </c>
+      <c r="M85" t="s">
         <v>173</v>
-      </c>
-      <c r="H85" t="s">
-        <v>171</v>
-      </c>
-      <c r="K85" t="s">
-        <v>200</v>
-      </c>
-      <c r="L85" t="s">
-        <v>188</v>
-      </c>
-      <c r="M85" t="s">
-        <v>192</v>
       </c>
       <c r="N85">
         <v>4</v>
@@ -4827,15 +4761,15 @@
         <v>5</v>
       </c>
       <c r="P85" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="B86" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C86" t="s">
         <v>68</v>
@@ -4850,28 +4784,29 @@
         <v>69</v>
       </c>
       <c r="G86" t="s">
+        <v>154</v>
+      </c>
+      <c r="H86" t="s">
+        <v>152</v>
+      </c>
+      <c r="K86" t="s">
+        <v>170</v>
+      </c>
+      <c r="L86" t="s">
+        <v>168</v>
+      </c>
+      <c r="M86" t="s">
         <v>173</v>
       </c>
-      <c r="H86" t="s">
-        <v>171</v>
-      </c>
-      <c r="K86" t="s">
-        <v>189</v>
-      </c>
-      <c r="L86" t="s">
-        <v>187</v>
-      </c>
-      <c r="M86" t="s">
-        <v>192</v>
-      </c>
       <c r="P86" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="S86" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>